<commit_message>
update ifrs sme model, add new image relative notes
</commit_message>
<xml_diff>
--- a/ifrs-sme-model.xlsx
+++ b/ifrs-sme-model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben.bravi\Documents\GitHub\IFRS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F0D18EF-B99F-4E87-9671-2E7066B2444B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B9E44F2-1CBA-4A40-8A65-7669520C14CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="692" activeTab="4" xr2:uid="{8907ADCE-C3F1-4516-963F-08DDED88069F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" tabRatio="692" firstSheet="3" activeTab="5" xr2:uid="{8907ADCE-C3F1-4516-963F-08DDED88069F}"/>
   </bookViews>
   <sheets>
     <sheet name="General information" sheetId="7" r:id="rId1"/>
@@ -2308,7 +2308,7 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="277">
+  <cellXfs count="275">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2614,6 +2614,33 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="14" fontId="5" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2632,15 +2659,6 @@
     <xf numFmtId="14" fontId="5" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="14" fontId="5" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2650,22 +2668,49 @@
     <xf numFmtId="14" fontId="5" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2674,10 +2719,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2689,67 +2752,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2758,15 +2767,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2785,10 +2785,19 @@
     <xf numFmtId="49" fontId="10" fillId="4" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2809,20 +2818,26 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2840,27 +2855,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3811,7 +3805,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:G2"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3822,119 +3816,119 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="203" t="s">
+      <c r="A1" s="191" t="s">
         <v>409</v>
       </c>
-      <c r="B1" s="204"/>
-      <c r="C1" s="204"/>
-      <c r="D1" s="204"/>
-      <c r="E1" s="204"/>
-      <c r="F1" s="204"/>
-      <c r="G1" s="205"/>
+      <c r="B1" s="192"/>
+      <c r="C1" s="192"/>
+      <c r="D1" s="192"/>
+      <c r="E1" s="192"/>
+      <c r="F1" s="192"/>
+      <c r="G1" s="193"/>
     </row>
     <row r="2" spans="1:7" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="136" t="s">
         <v>423</v>
       </c>
-      <c r="B2" s="197" t="s">
+      <c r="B2" s="194" t="s">
         <v>430</v>
       </c>
-      <c r="C2" s="198"/>
-      <c r="D2" s="198"/>
-      <c r="E2" s="198"/>
-      <c r="F2" s="198"/>
-      <c r="G2" s="199"/>
+      <c r="C2" s="195"/>
+      <c r="D2" s="195"/>
+      <c r="E2" s="195"/>
+      <c r="F2" s="195"/>
+      <c r="G2" s="196"/>
     </row>
     <row r="3" spans="1:7" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="136" t="s">
         <v>426</v>
       </c>
-      <c r="B3" s="197" t="s">
+      <c r="B3" s="194" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="198"/>
-      <c r="D3" s="198"/>
-      <c r="E3" s="198"/>
-      <c r="F3" s="198"/>
-      <c r="G3" s="199"/>
+      <c r="C3" s="195"/>
+      <c r="D3" s="195"/>
+      <c r="E3" s="195"/>
+      <c r="F3" s="195"/>
+      <c r="G3" s="196"/>
     </row>
     <row r="4" spans="1:7" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="136" t="s">
         <v>424</v>
       </c>
-      <c r="B4" s="197" t="s">
+      <c r="B4" s="194" t="s">
         <v>425</v>
       </c>
-      <c r="C4" s="198"/>
-      <c r="D4" s="198"/>
-      <c r="E4" s="198"/>
-      <c r="F4" s="198"/>
-      <c r="G4" s="199"/>
+      <c r="C4" s="195"/>
+      <c r="D4" s="195"/>
+      <c r="E4" s="195"/>
+      <c r="F4" s="195"/>
+      <c r="G4" s="196"/>
     </row>
     <row r="5" spans="1:7" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="136" t="s">
         <v>551</v>
       </c>
-      <c r="B5" s="197" t="s">
+      <c r="B5" s="194" t="s">
         <v>554</v>
       </c>
-      <c r="C5" s="198"/>
-      <c r="D5" s="198"/>
-      <c r="E5" s="198"/>
-      <c r="F5" s="198"/>
-      <c r="G5" s="199"/>
+      <c r="C5" s="195"/>
+      <c r="D5" s="195"/>
+      <c r="E5" s="195"/>
+      <c r="F5" s="195"/>
+      <c r="G5" s="196"/>
     </row>
     <row r="6" spans="1:7" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="136" t="s">
         <v>422</v>
       </c>
-      <c r="B6" s="197" t="s">
+      <c r="B6" s="194" t="s">
         <v>431</v>
       </c>
-      <c r="C6" s="198"/>
-      <c r="D6" s="198"/>
-      <c r="E6" s="198"/>
-      <c r="F6" s="198"/>
-      <c r="G6" s="199"/>
+      <c r="C6" s="195"/>
+      <c r="D6" s="195"/>
+      <c r="E6" s="195"/>
+      <c r="F6" s="195"/>
+      <c r="G6" s="196"/>
     </row>
     <row r="7" spans="1:7" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="136" t="s">
         <v>552</v>
       </c>
-      <c r="B7" s="197" t="s">
+      <c r="B7" s="194" t="s">
         <v>555</v>
       </c>
-      <c r="C7" s="198"/>
-      <c r="D7" s="198"/>
-      <c r="E7" s="198"/>
-      <c r="F7" s="198"/>
-      <c r="G7" s="199"/>
+      <c r="C7" s="195"/>
+      <c r="D7" s="195"/>
+      <c r="E7" s="195"/>
+      <c r="F7" s="195"/>
+      <c r="G7" s="196"/>
     </row>
     <row r="8" spans="1:7" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A8" s="136" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="206">
+      <c r="B8" s="197">
         <v>45291</v>
       </c>
-      <c r="C8" s="207"/>
-      <c r="D8" s="207"/>
-      <c r="E8" s="207"/>
-      <c r="F8" s="207"/>
-      <c r="G8" s="208"/>
+      <c r="C8" s="198"/>
+      <c r="D8" s="198"/>
+      <c r="E8" s="198"/>
+      <c r="F8" s="198"/>
+      <c r="G8" s="199"/>
     </row>
     <row r="9" spans="1:7" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A9" s="155" t="s">
         <v>81</v>
       </c>
-      <c r="B9" s="191">
+      <c r="B9" s="200">
         <v>45657</v>
       </c>
-      <c r="C9" s="192"/>
-      <c r="D9" s="192"/>
-      <c r="E9" s="192"/>
-      <c r="F9" s="192"/>
-      <c r="G9" s="193"/>
+      <c r="C9" s="201"/>
+      <c r="D9" s="201"/>
+      <c r="E9" s="201"/>
+      <c r="F9" s="201"/>
+      <c r="G9" s="202"/>
     </row>
     <row r="10" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="151" t="s">
@@ -3980,125 +3974,120 @@
       <c r="A14" s="134" t="s">
         <v>410</v>
       </c>
-      <c r="B14" s="191" t="s">
+      <c r="B14" s="200" t="s">
         <v>412</v>
       </c>
-      <c r="C14" s="192"/>
-      <c r="D14" s="192"/>
-      <c r="E14" s="192"/>
-      <c r="F14" s="192"/>
-      <c r="G14" s="193"/>
+      <c r="C14" s="201"/>
+      <c r="D14" s="201"/>
+      <c r="E14" s="201"/>
+      <c r="F14" s="201"/>
+      <c r="G14" s="202"/>
     </row>
     <row r="15" spans="1:7" ht="18" x14ac:dyDescent="0.4">
       <c r="A15" s="134"/>
-      <c r="B15" s="191" t="s">
+      <c r="B15" s="200" t="s">
         <v>413</v>
       </c>
-      <c r="C15" s="192"/>
-      <c r="D15" s="192"/>
-      <c r="E15" s="192"/>
-      <c r="F15" s="192"/>
-      <c r="G15" s="193"/>
+      <c r="C15" s="201"/>
+      <c r="D15" s="201"/>
+      <c r="E15" s="201"/>
+      <c r="F15" s="201"/>
+      <c r="G15" s="202"/>
     </row>
     <row r="16" spans="1:7" ht="18" x14ac:dyDescent="0.4">
       <c r="A16" s="134"/>
-      <c r="B16" s="191" t="s">
+      <c r="B16" s="200" t="s">
         <v>414</v>
       </c>
-      <c r="C16" s="192"/>
-      <c r="D16" s="192"/>
-      <c r="E16" s="192"/>
-      <c r="F16" s="192"/>
-      <c r="G16" s="193"/>
+      <c r="C16" s="201"/>
+      <c r="D16" s="201"/>
+      <c r="E16" s="201"/>
+      <c r="F16" s="201"/>
+      <c r="G16" s="202"/>
     </row>
     <row r="17" spans="1:7" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A17" s="135"/>
-      <c r="B17" s="194" t="s">
+      <c r="B17" s="203" t="s">
         <v>415</v>
       </c>
-      <c r="C17" s="195"/>
-      <c r="D17" s="195"/>
-      <c r="E17" s="195"/>
-      <c r="F17" s="195"/>
-      <c r="G17" s="196"/>
+      <c r="C17" s="204"/>
+      <c r="D17" s="204"/>
+      <c r="E17" s="204"/>
+      <c r="F17" s="204"/>
+      <c r="G17" s="205"/>
     </row>
     <row r="18" spans="1:7" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A18" s="134" t="s">
         <v>411</v>
       </c>
-      <c r="B18" s="191" t="s">
+      <c r="B18" s="200" t="s">
         <v>416</v>
       </c>
-      <c r="C18" s="192"/>
-      <c r="D18" s="192"/>
-      <c r="E18" s="192"/>
-      <c r="F18" s="192"/>
-      <c r="G18" s="193"/>
+      <c r="C18" s="201"/>
+      <c r="D18" s="201"/>
+      <c r="E18" s="201"/>
+      <c r="F18" s="201"/>
+      <c r="G18" s="202"/>
     </row>
     <row r="19" spans="1:7" ht="18" x14ac:dyDescent="0.4">
       <c r="A19" s="133" t="s">
         <v>417</v>
       </c>
-      <c r="B19" s="200" t="s">
+      <c r="B19" s="206" t="s">
         <v>418</v>
       </c>
-      <c r="C19" s="201"/>
-      <c r="D19" s="201"/>
-      <c r="E19" s="201"/>
-      <c r="F19" s="201"/>
-      <c r="G19" s="202"/>
+      <c r="C19" s="207"/>
+      <c r="D19" s="207"/>
+      <c r="E19" s="207"/>
+      <c r="F19" s="207"/>
+      <c r="G19" s="208"/>
     </row>
     <row r="20" spans="1:7" ht="18" x14ac:dyDescent="0.4">
       <c r="A20" s="134"/>
-      <c r="B20" s="191" t="s">
+      <c r="B20" s="200" t="s">
         <v>419</v>
       </c>
-      <c r="C20" s="192"/>
-      <c r="D20" s="192"/>
-      <c r="E20" s="192"/>
-      <c r="F20" s="192"/>
-      <c r="G20" s="193"/>
+      <c r="C20" s="201"/>
+      <c r="D20" s="201"/>
+      <c r="E20" s="201"/>
+      <c r="F20" s="201"/>
+      <c r="G20" s="202"/>
     </row>
     <row r="21" spans="1:7" ht="18" x14ac:dyDescent="0.4">
       <c r="A21" s="134"/>
-      <c r="B21" s="191" t="s">
+      <c r="B21" s="200" t="s">
         <v>389</v>
       </c>
-      <c r="C21" s="192"/>
-      <c r="D21" s="192"/>
-      <c r="E21" s="192"/>
-      <c r="F21" s="192"/>
-      <c r="G21" s="193"/>
+      <c r="C21" s="201"/>
+      <c r="D21" s="201"/>
+      <c r="E21" s="201"/>
+      <c r="F21" s="201"/>
+      <c r="G21" s="202"/>
     </row>
     <row r="22" spans="1:7" ht="18" x14ac:dyDescent="0.4">
       <c r="A22" s="134"/>
-      <c r="B22" s="191" t="s">
+      <c r="B22" s="200" t="s">
         <v>420</v>
       </c>
-      <c r="C22" s="192"/>
-      <c r="D22" s="192"/>
-      <c r="E22" s="192"/>
-      <c r="F22" s="192"/>
-      <c r="G22" s="193"/>
+      <c r="C22" s="201"/>
+      <c r="D22" s="201"/>
+      <c r="E22" s="201"/>
+      <c r="F22" s="201"/>
+      <c r="G22" s="202"/>
     </row>
     <row r="23" spans="1:7" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A23" s="135"/>
-      <c r="B23" s="194" t="s">
+      <c r="B23" s="203" t="s">
         <v>421</v>
       </c>
-      <c r="C23" s="195"/>
-      <c r="D23" s="195"/>
-      <c r="E23" s="195"/>
-      <c r="F23" s="195"/>
-      <c r="G23" s="196"/>
+      <c r="C23" s="204"/>
+      <c r="D23" s="204"/>
+      <c r="E23" s="204"/>
+      <c r="F23" s="204"/>
+      <c r="G23" s="205"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
     <mergeCell ref="B21:G21"/>
     <mergeCell ref="B22:G22"/>
     <mergeCell ref="B23:G23"/>
@@ -4113,6 +4102,11 @@
     <mergeCell ref="B20:G20"/>
     <mergeCell ref="B14:G14"/>
     <mergeCell ref="B7:G7"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="41" orientation="portrait" r:id="rId1"/>
@@ -4128,7 +4122,7 @@
   <dimension ref="A1:G103"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B10" sqref="B10:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -4137,7 +4131,7 @@
     <col min="2" max="2" width="111.1796875" style="2" customWidth="1"/>
     <col min="3" max="3" width="7.08984375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="2" customWidth="1"/>
-    <col min="5" max="6" width="11.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.7265625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26.54296875" style="41" customWidth="1"/>
     <col min="8" max="19" width="8.7265625" style="2"/>
     <col min="20" max="20" width="7" style="2" customWidth="1"/>
@@ -4146,118 +4140,118 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="203" t="s">
+      <c r="A1" s="191" t="s">
         <v>407</v>
       </c>
-      <c r="B1" s="204"/>
-      <c r="C1" s="204"/>
-      <c r="D1" s="204"/>
-      <c r="E1" s="204"/>
-      <c r="F1" s="204"/>
-      <c r="G1" s="205"/>
+      <c r="B1" s="192"/>
+      <c r="C1" s="192"/>
+      <c r="D1" s="192"/>
+      <c r="E1" s="192"/>
+      <c r="F1" s="192"/>
+      <c r="G1" s="193"/>
     </row>
     <row r="2" spans="1:7" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="136" t="s">
         <v>423</v>
       </c>
-      <c r="B2" s="231" t="str">
+      <c r="B2" s="209" t="str">
         <f>'General information'!B2</f>
         <v>CompanyName LegalForm</v>
       </c>
-      <c r="C2" s="232"/>
-      <c r="D2" s="232"/>
-      <c r="E2" s="232"/>
-      <c r="F2" s="232"/>
-      <c r="G2" s="233"/>
+      <c r="C2" s="210"/>
+      <c r="D2" s="210"/>
+      <c r="E2" s="210"/>
+      <c r="F2" s="210"/>
+      <c r="G2" s="211"/>
     </row>
     <row r="3" spans="1:7" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="140" t="s">
         <v>426</v>
       </c>
-      <c r="B3" s="231" t="str">
+      <c r="B3" s="209" t="str">
         <f>'General information'!B3</f>
         <v>Address 1234, Country</v>
       </c>
-      <c r="C3" s="232"/>
-      <c r="D3" s="232"/>
-      <c r="E3" s="232"/>
-      <c r="F3" s="232"/>
-      <c r="G3" s="233"/>
+      <c r="C3" s="210"/>
+      <c r="D3" s="210"/>
+      <c r="E3" s="210"/>
+      <c r="F3" s="210"/>
+      <c r="G3" s="211"/>
     </row>
     <row r="4" spans="1:7" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="136" t="s">
         <v>80</v>
       </c>
-      <c r="B4" s="191">
+      <c r="B4" s="200">
         <f>'General information'!B8</f>
         <v>45291</v>
       </c>
-      <c r="C4" s="192"/>
-      <c r="D4" s="192"/>
-      <c r="E4" s="192"/>
-      <c r="F4" s="192"/>
-      <c r="G4" s="193"/>
+      <c r="C4" s="201"/>
+      <c r="D4" s="201"/>
+      <c r="E4" s="201"/>
+      <c r="F4" s="201"/>
+      <c r="G4" s="202"/>
     </row>
     <row r="5" spans="1:7" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="136" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="191">
+      <c r="B5" s="200">
         <f>'General information'!B9</f>
         <v>45657</v>
       </c>
-      <c r="C5" s="192"/>
-      <c r="D5" s="192"/>
-      <c r="E5" s="192"/>
-      <c r="F5" s="192"/>
-      <c r="G5" s="193"/>
+      <c r="C5" s="201"/>
+      <c r="D5" s="201"/>
+      <c r="E5" s="201"/>
+      <c r="F5" s="201"/>
+      <c r="G5" s="202"/>
     </row>
     <row r="6" spans="1:7" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="203" t="s">
+      <c r="A6" s="191" t="s">
         <v>406</v>
       </c>
-      <c r="B6" s="204"/>
-      <c r="C6" s="204"/>
-      <c r="D6" s="204"/>
-      <c r="E6" s="204"/>
-      <c r="F6" s="204"/>
-      <c r="G6" s="205"/>
+      <c r="B6" s="192"/>
+      <c r="C6" s="192"/>
+      <c r="D6" s="192"/>
+      <c r="E6" s="192"/>
+      <c r="F6" s="192"/>
+      <c r="G6" s="193"/>
     </row>
     <row r="7" spans="1:7" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="127" t="s">
         <v>90</v>
       </c>
-      <c r="B7" s="226" t="s">
+      <c r="B7" s="231" t="s">
         <v>89</v>
       </c>
-      <c r="C7" s="227"/>
-      <c r="D7" s="227"/>
-      <c r="E7" s="227"/>
-      <c r="F7" s="227"/>
-      <c r="G7" s="228"/>
+      <c r="C7" s="232"/>
+      <c r="D7" s="232"/>
+      <c r="E7" s="232"/>
+      <c r="F7" s="232"/>
+      <c r="G7" s="233"/>
     </row>
     <row r="8" spans="1:7" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A8" s="114" t="s">
         <v>282</v>
       </c>
-      <c r="B8" s="234" t="s">
+      <c r="B8" s="212" t="s">
         <v>579</v>
       </c>
-      <c r="C8" s="235"/>
-      <c r="D8" s="235"/>
-      <c r="E8" s="235"/>
-      <c r="F8" s="235"/>
-      <c r="G8" s="236"/>
+      <c r="C8" s="213"/>
+      <c r="D8" s="213"/>
+      <c r="E8" s="213"/>
+      <c r="F8" s="213"/>
+      <c r="G8" s="214"/>
     </row>
     <row r="9" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="10" spans="1:7" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A10" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="B10" s="224" t="s">
+      <c r="B10" s="229" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="225"/>
+      <c r="C10" s="230"/>
       <c r="D10" s="179" t="s">
         <v>73</v>
       </c>
@@ -4274,33 +4268,33 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="216" t="s">
+      <c r="B11" s="215" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="217"/>
-      <c r="D11" s="217"/>
-      <c r="E11" s="217"/>
-      <c r="F11" s="217"/>
-      <c r="G11" s="218"/>
+      <c r="C11" s="216"/>
+      <c r="D11" s="216"/>
+      <c r="E11" s="216"/>
+      <c r="F11" s="216"/>
+      <c r="G11" s="217"/>
     </row>
     <row r="12" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="221" t="s">
+      <c r="B12" s="226" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="222"/>
-      <c r="D12" s="222"/>
-      <c r="E12" s="222"/>
-      <c r="F12" s="222"/>
-      <c r="G12" s="223"/>
+      <c r="C12" s="227"/>
+      <c r="D12" s="227"/>
+      <c r="E12" s="227"/>
+      <c r="F12" s="227"/>
+      <c r="G12" s="228"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="B13" s="219" t="s">
+      <c r="B13" s="218" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="220"/>
+      <c r="C13" s="219"/>
       <c r="D13" s="7" t="s">
         <v>123</v>
       </c>
@@ -4318,10 +4312,10 @@
       <c r="A14" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="B14" s="211" t="s">
+      <c r="B14" s="220" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="212"/>
+      <c r="C14" s="221"/>
       <c r="D14" s="8"/>
       <c r="E14" s="81"/>
       <c r="F14" s="87">
@@ -4333,10 +4327,10 @@
       <c r="A15" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="B15" s="211" t="s">
+      <c r="B15" s="220" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="212"/>
+      <c r="C15" s="221"/>
       <c r="D15" s="8"/>
       <c r="E15" s="81"/>
       <c r="F15" s="87"/>
@@ -4346,10 +4340,10 @@
       <c r="A16" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="B16" s="211" t="s">
+      <c r="B16" s="220" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="212"/>
+      <c r="C16" s="221"/>
       <c r="D16" s="8"/>
       <c r="E16" s="81">
         <v>20</v>
@@ -4363,10 +4357,10 @@
       <c r="A17" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="B17" s="211" t="s">
+      <c r="B17" s="220" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="212"/>
+      <c r="C17" s="221"/>
       <c r="D17" s="8"/>
       <c r="E17" s="81">
         <v>30</v>
@@ -4380,10 +4374,10 @@
       <c r="A18" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="B18" s="211" t="s">
+      <c r="B18" s="220" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="212"/>
+      <c r="C18" s="221"/>
       <c r="D18" s="8"/>
       <c r="E18" s="81"/>
       <c r="F18" s="87"/>
@@ -4393,10 +4387,10 @@
       <c r="A19" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="B19" s="211" t="s">
+      <c r="B19" s="220" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="212"/>
+      <c r="C19" s="221"/>
       <c r="D19" s="8"/>
       <c r="E19" s="81"/>
       <c r="F19" s="87"/>
@@ -4406,10 +4400,10 @@
       <c r="A20" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="B20" s="211" t="s">
+      <c r="B20" s="220" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="212"/>
+      <c r="C20" s="221"/>
       <c r="D20" s="8"/>
       <c r="E20" s="81"/>
       <c r="F20" s="87"/>
@@ -4419,10 +4413,10 @@
       <c r="A21" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="B21" s="211" t="s">
+      <c r="B21" s="220" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="212"/>
+      <c r="C21" s="221"/>
       <c r="D21" s="8"/>
       <c r="E21" s="81"/>
       <c r="F21" s="87"/>
@@ -4432,10 +4426,10 @@
       <c r="A22" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="B22" s="211" t="s">
+      <c r="B22" s="220" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="212"/>
+      <c r="C22" s="221"/>
       <c r="D22" s="8" t="s">
         <v>124</v>
       </c>
@@ -4449,10 +4443,10 @@
       <c r="A23" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="B23" s="211" t="s">
+      <c r="B23" s="220" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="212"/>
+      <c r="C23" s="221"/>
       <c r="D23" s="8" t="s">
         <v>125</v>
       </c>
@@ -4466,10 +4460,10 @@
       <c r="A24" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="B24" s="211" t="s">
+      <c r="B24" s="220" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="212"/>
+      <c r="C24" s="221"/>
       <c r="D24" s="8"/>
       <c r="E24" s="81"/>
       <c r="F24" s="87"/>
@@ -4479,10 +4473,10 @@
       <c r="A25" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="B25" s="211" t="s">
+      <c r="B25" s="220" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="212"/>
+      <c r="C25" s="221"/>
       <c r="D25" s="8"/>
       <c r="E25" s="81"/>
       <c r="F25" s="87"/>
@@ -4492,10 +4486,10 @@
       <c r="A26" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="B26" s="211" t="s">
+      <c r="B26" s="220" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="212"/>
+      <c r="C26" s="221"/>
       <c r="D26" s="8"/>
       <c r="E26" s="81"/>
       <c r="F26" s="87"/>
@@ -4505,20 +4499,20 @@
       <c r="A27" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="B27" s="209" t="s">
+      <c r="B27" s="224" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="210"/>
+      <c r="C27" s="225"/>
       <c r="D27" s="9"/>
       <c r="E27" s="88"/>
       <c r="F27" s="87"/>
       <c r="G27" s="46"/>
     </row>
     <row r="28" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="229" t="s">
+      <c r="B28" s="222" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="230"/>
+      <c r="C28" s="223"/>
       <c r="E28" s="84">
         <f>SUM(E13:E27)</f>
         <v>104</v>
@@ -4546,23 +4540,23 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="216" t="s">
+      <c r="B31" s="215" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="217"/>
-      <c r="D31" s="217"/>
-      <c r="E31" s="217"/>
-      <c r="F31" s="217"/>
-      <c r="G31" s="217"/>
+      <c r="C31" s="216"/>
+      <c r="D31" s="216"/>
+      <c r="E31" s="216"/>
+      <c r="F31" s="216"/>
+      <c r="G31" s="216"/>
     </row>
     <row r="32" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="B32" s="219" t="s">
+      <c r="B32" s="218" t="s">
         <v>2</v>
       </c>
-      <c r="C32" s="220"/>
+      <c r="C32" s="219"/>
       <c r="D32" s="7" t="s">
         <v>126</v>
       </c>
@@ -4580,10 +4574,10 @@
       <c r="A33" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="B33" s="211" t="s">
+      <c r="B33" s="220" t="s">
         <v>3</v>
       </c>
-      <c r="C33" s="212"/>
+      <c r="C33" s="221"/>
       <c r="D33" s="8" t="s">
         <v>127</v>
       </c>
@@ -4597,10 +4591,10 @@
       <c r="A34" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="B34" s="211" t="s">
+      <c r="B34" s="220" t="s">
         <v>4</v>
       </c>
-      <c r="C34" s="212"/>
+      <c r="C34" s="221"/>
       <c r="D34" s="8"/>
       <c r="E34" s="81"/>
       <c r="F34" s="81"/>
@@ -4610,10 +4604,10 @@
       <c r="A35" s="26" t="s">
         <v>110</v>
       </c>
-      <c r="B35" s="211" t="s">
+      <c r="B35" s="220" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="212"/>
+      <c r="C35" s="221"/>
       <c r="D35" s="8"/>
       <c r="E35" s="81"/>
       <c r="F35" s="81"/>
@@ -4623,10 +4617,10 @@
       <c r="A36" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="B36" s="211" t="s">
+      <c r="B36" s="220" t="s">
         <v>6</v>
       </c>
-      <c r="C36" s="212"/>
+      <c r="C36" s="221"/>
       <c r="D36" s="8"/>
       <c r="E36" s="81"/>
       <c r="F36" s="81"/>
@@ -4636,10 +4630,10 @@
       <c r="A37" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="B37" s="211" t="s">
+      <c r="B37" s="220" t="s">
         <v>7</v>
       </c>
-      <c r="C37" s="212"/>
+      <c r="C37" s="221"/>
       <c r="D37" s="8"/>
       <c r="E37" s="81"/>
       <c r="F37" s="81"/>
@@ -4649,10 +4643,10 @@
       <c r="A38" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="B38" s="211" t="s">
+      <c r="B38" s="220" t="s">
         <v>8</v>
       </c>
-      <c r="C38" s="212"/>
+      <c r="C38" s="221"/>
       <c r="D38" s="8"/>
       <c r="E38" s="81"/>
       <c r="F38" s="81"/>
@@ -4662,10 +4656,10 @@
       <c r="A39" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="B39" s="211" t="s">
+      <c r="B39" s="220" t="s">
         <v>9</v>
       </c>
-      <c r="C39" s="212"/>
+      <c r="C39" s="221"/>
       <c r="D39" s="8"/>
       <c r="E39" s="81">
         <v>10</v>
@@ -4679,20 +4673,20 @@
       <c r="A40" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="B40" s="209" t="s">
+      <c r="B40" s="224" t="s">
         <v>10</v>
       </c>
-      <c r="C40" s="210"/>
+      <c r="C40" s="225"/>
       <c r="D40" s="9"/>
       <c r="E40" s="88"/>
       <c r="F40" s="88"/>
       <c r="G40" s="46"/>
     </row>
     <row r="41" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="216" t="s">
+      <c r="B41" s="215" t="s">
         <v>30</v>
       </c>
-      <c r="C41" s="218"/>
+      <c r="C41" s="217"/>
       <c r="E41" s="89">
         <f>SUM(E32:E40)</f>
         <v>40</v>
@@ -4703,10 +4697,10 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="216" t="s">
+      <c r="B42" s="215" t="s">
         <v>31</v>
       </c>
-      <c r="C42" s="218"/>
+      <c r="C42" s="217"/>
       <c r="E42" s="89">
         <f>SUM(E28,E41)</f>
         <v>144</v>
@@ -4737,33 +4731,33 @@
       </c>
     </row>
     <row r="45" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="216" t="s">
+      <c r="B45" s="215" t="s">
         <v>32</v>
       </c>
-      <c r="C45" s="217"/>
-      <c r="D45" s="217"/>
-      <c r="E45" s="217"/>
-      <c r="F45" s="217"/>
-      <c r="G45" s="218"/>
+      <c r="C45" s="216"/>
+      <c r="D45" s="216"/>
+      <c r="E45" s="216"/>
+      <c r="F45" s="216"/>
+      <c r="G45" s="217"/>
     </row>
     <row r="46" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="216" t="s">
+      <c r="B46" s="215" t="s">
         <v>33</v>
       </c>
-      <c r="C46" s="217"/>
-      <c r="D46" s="217"/>
-      <c r="E46" s="217"/>
-      <c r="F46" s="217"/>
-      <c r="G46" s="218"/>
+      <c r="C46" s="216"/>
+      <c r="D46" s="216"/>
+      <c r="E46" s="216"/>
+      <c r="F46" s="216"/>
+      <c r="G46" s="217"/>
     </row>
     <row r="47" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="B47" s="219" t="s">
+      <c r="B47" s="218" t="s">
         <v>34</v>
       </c>
-      <c r="C47" s="220"/>
+      <c r="C47" s="219"/>
       <c r="D47" s="7" t="s">
         <v>128</v>
       </c>
@@ -4777,10 +4771,10 @@
       <c r="A48" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="B48" s="211" t="s">
+      <c r="B48" s="220" t="s">
         <v>35</v>
       </c>
-      <c r="C48" s="212"/>
+      <c r="C48" s="221"/>
       <c r="D48" s="8" t="s">
         <v>129</v>
       </c>
@@ -4794,10 +4788,10 @@
       <c r="A49" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="B49" s="211" t="s">
+      <c r="B49" s="220" t="s">
         <v>36</v>
       </c>
-      <c r="C49" s="212"/>
+      <c r="C49" s="221"/>
       <c r="D49" s="8" t="s">
         <v>130</v>
       </c>
@@ -4811,10 +4805,10 @@
       <c r="A50" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="B50" s="211" t="s">
+      <c r="B50" s="220" t="s">
         <v>37</v>
       </c>
-      <c r="C50" s="212"/>
+      <c r="C50" s="221"/>
       <c r="D50" s="8"/>
       <c r="E50" s="81"/>
       <c r="F50" s="87"/>
@@ -4824,10 +4818,10 @@
       <c r="A51" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="B51" s="211" t="s">
+      <c r="B51" s="220" t="s">
         <v>38</v>
       </c>
-      <c r="C51" s="212"/>
+      <c r="C51" s="221"/>
       <c r="D51" s="8" t="s">
         <v>131</v>
       </c>
@@ -4841,10 +4835,10 @@
       <c r="A52" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="B52" s="211" t="s">
+      <c r="B52" s="220" t="s">
         <v>39</v>
       </c>
-      <c r="C52" s="212"/>
+      <c r="C52" s="221"/>
       <c r="D52" s="9" t="s">
         <v>132</v>
       </c>
@@ -4860,10 +4854,10 @@
     </row>
     <row r="53" spans="1:7" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="3"/>
-      <c r="B53" s="216" t="s">
+      <c r="B53" s="215" t="s">
         <v>40</v>
       </c>
-      <c r="C53" s="218"/>
+      <c r="C53" s="217"/>
       <c r="D53" s="90"/>
       <c r="E53" s="92">
         <f>SUM(E47:E52)</f>
@@ -4878,19 +4872,19 @@
       <c r="A54" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="B54" s="209" t="s">
+      <c r="B54" s="224" t="s">
         <v>41</v>
       </c>
-      <c r="C54" s="210"/>
+      <c r="C54" s="225"/>
       <c r="D54" s="91"/>
       <c r="E54" s="10"/>
       <c r="F54" s="11"/>
     </row>
     <row r="55" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B55" s="216" t="s">
+      <c r="B55" s="215" t="s">
         <v>42</v>
       </c>
-      <c r="C55" s="218"/>
+      <c r="C55" s="217"/>
       <c r="E55" s="84">
         <f>SUM(E53,E54)</f>
         <v>15</v>
@@ -4918,33 +4912,33 @@
       </c>
     </row>
     <row r="58" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="216" t="s">
+      <c r="B58" s="215" t="s">
         <v>43</v>
       </c>
-      <c r="C58" s="217"/>
-      <c r="D58" s="217"/>
-      <c r="E58" s="217"/>
-      <c r="F58" s="217"/>
-      <c r="G58" s="218"/>
+      <c r="C58" s="216"/>
+      <c r="D58" s="216"/>
+      <c r="E58" s="216"/>
+      <c r="F58" s="216"/>
+      <c r="G58" s="217"/>
     </row>
     <row r="59" spans="1:7" ht="14.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="221" t="s">
+      <c r="B59" s="226" t="s">
         <v>44</v>
       </c>
-      <c r="C59" s="222"/>
-      <c r="D59" s="222"/>
-      <c r="E59" s="222"/>
-      <c r="F59" s="222"/>
-      <c r="G59" s="222"/>
+      <c r="C59" s="227"/>
+      <c r="D59" s="227"/>
+      <c r="E59" s="227"/>
+      <c r="F59" s="227"/>
+      <c r="G59" s="227"/>
     </row>
     <row r="60" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="25" t="s">
         <v>295</v>
       </c>
-      <c r="B60" s="219" t="s">
+      <c r="B60" s="218" t="s">
         <v>45</v>
       </c>
-      <c r="C60" s="220"/>
+      <c r="C60" s="219"/>
       <c r="D60" s="7"/>
       <c r="E60" s="85"/>
       <c r="F60" s="86"/>
@@ -4954,10 +4948,10 @@
       <c r="A61" s="26" t="s">
         <v>296</v>
       </c>
-      <c r="B61" s="211" t="s">
+      <c r="B61" s="220" t="s">
         <v>46</v>
       </c>
-      <c r="C61" s="212"/>
+      <c r="C61" s="221"/>
       <c r="D61" s="8" t="s">
         <v>313</v>
       </c>
@@ -4975,10 +4969,10 @@
       <c r="A62" s="27" t="s">
         <v>297</v>
       </c>
-      <c r="B62" s="209" t="s">
+      <c r="B62" s="224" t="s">
         <v>47</v>
       </c>
-      <c r="C62" s="210"/>
+      <c r="C62" s="225"/>
       <c r="D62" s="9"/>
       <c r="E62" s="88">
         <v>2</v>
@@ -5007,10 +5001,10 @@
       <c r="A64" s="25" t="s">
         <v>298</v>
       </c>
-      <c r="B64" s="219" t="s">
+      <c r="B64" s="218" t="s">
         <v>49</v>
       </c>
-      <c r="C64" s="220"/>
+      <c r="C64" s="219"/>
       <c r="D64" s="7" t="s">
         <v>314</v>
       </c>
@@ -5024,10 +5018,10 @@
       <c r="A65" s="26" t="s">
         <v>299</v>
       </c>
-      <c r="B65" s="211" t="s">
+      <c r="B65" s="220" t="s">
         <v>50</v>
       </c>
-      <c r="C65" s="212"/>
+      <c r="C65" s="221"/>
       <c r="D65" s="8"/>
       <c r="E65" s="81">
         <v>4</v>
@@ -5041,10 +5035,10 @@
       <c r="A66" s="26" t="s">
         <v>300</v>
       </c>
-      <c r="B66" s="211" t="s">
+      <c r="B66" s="220" t="s">
         <v>51</v>
       </c>
-      <c r="C66" s="212"/>
+      <c r="C66" s="221"/>
       <c r="D66" s="8"/>
       <c r="E66" s="81"/>
       <c r="F66" s="87"/>
@@ -5054,10 +5048,10 @@
       <c r="A67" s="26" t="s">
         <v>301</v>
       </c>
-      <c r="B67" s="211" t="s">
+      <c r="B67" s="220" t="s">
         <v>52</v>
       </c>
-      <c r="C67" s="212"/>
+      <c r="C67" s="221"/>
       <c r="D67" s="8"/>
       <c r="E67" s="81"/>
       <c r="F67" s="87"/>
@@ -5067,10 +5061,10 @@
       <c r="A68" s="26" t="s">
         <v>302</v>
       </c>
-      <c r="B68" s="211" t="s">
+      <c r="B68" s="220" t="s">
         <v>53</v>
       </c>
-      <c r="C68" s="212"/>
+      <c r="C68" s="221"/>
       <c r="D68" s="8"/>
       <c r="E68" s="81"/>
       <c r="F68" s="87"/>
@@ -5080,20 +5074,20 @@
       <c r="A69" s="27" t="s">
         <v>303</v>
       </c>
-      <c r="B69" s="209" t="s">
+      <c r="B69" s="224" t="s">
         <v>54</v>
       </c>
-      <c r="C69" s="210"/>
+      <c r="C69" s="225"/>
       <c r="D69" s="9"/>
       <c r="E69" s="88"/>
       <c r="F69" s="94"/>
       <c r="G69" s="46"/>
     </row>
     <row r="70" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B70" s="216" t="s">
+      <c r="B70" s="215" t="s">
         <v>55</v>
       </c>
-      <c r="C70" s="218"/>
+      <c r="C70" s="217"/>
       <c r="E70" s="84">
         <f>SUM(E63:E69)</f>
         <v>9</v>
@@ -5122,23 +5116,23 @@
       </c>
     </row>
     <row r="73" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B73" s="216" t="s">
+      <c r="B73" s="215" t="s">
         <v>56</v>
       </c>
-      <c r="C73" s="217"/>
-      <c r="D73" s="217"/>
-      <c r="E73" s="217"/>
-      <c r="F73" s="217"/>
-      <c r="G73" s="217"/>
+      <c r="C73" s="216"/>
+      <c r="D73" s="216"/>
+      <c r="E73" s="216"/>
+      <c r="F73" s="216"/>
+      <c r="G73" s="216"/>
     </row>
     <row r="74" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="25" t="s">
         <v>304</v>
       </c>
-      <c r="B74" s="219" t="s">
+      <c r="B74" s="218" t="s">
         <v>57</v>
       </c>
-      <c r="C74" s="220"/>
+      <c r="C74" s="219"/>
       <c r="D74" s="7"/>
       <c r="E74" s="85"/>
       <c r="F74" s="87"/>
@@ -5148,10 +5142,10 @@
       <c r="A75" s="26" t="s">
         <v>305</v>
       </c>
-      <c r="B75" s="211" t="s">
+      <c r="B75" s="220" t="s">
         <v>58</v>
       </c>
-      <c r="C75" s="212"/>
+      <c r="C75" s="221"/>
       <c r="D75" s="8" t="s">
         <v>313</v>
       </c>
@@ -5169,20 +5163,20 @@
       <c r="A76" s="27" t="s">
         <v>306</v>
       </c>
-      <c r="B76" s="209" t="s">
+      <c r="B76" s="224" t="s">
         <v>59</v>
       </c>
-      <c r="C76" s="210"/>
+      <c r="C76" s="225"/>
       <c r="D76" s="9"/>
       <c r="E76" s="88"/>
       <c r="F76" s="87"/>
       <c r="G76" s="46"/>
     </row>
     <row r="77" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B77" s="216" t="s">
+      <c r="B77" s="215" t="s">
         <v>60</v>
       </c>
-      <c r="C77" s="218"/>
+      <c r="C77" s="217"/>
       <c r="D77" s="95"/>
       <c r="E77" s="82">
         <f>SUM(E74:E76)</f>
@@ -5197,10 +5191,10 @@
       <c r="A78" s="25" t="s">
         <v>307</v>
       </c>
-      <c r="B78" s="219" t="s">
+      <c r="B78" s="218" t="s">
         <v>61</v>
       </c>
-      <c r="C78" s="220"/>
+      <c r="C78" s="219"/>
       <c r="D78" s="7" t="s">
         <v>314</v>
       </c>
@@ -5218,10 +5212,10 @@
       <c r="A79" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="B79" s="211" t="s">
+      <c r="B79" s="220" t="s">
         <v>62</v>
       </c>
-      <c r="C79" s="212"/>
+      <c r="C79" s="221"/>
       <c r="D79" s="8"/>
       <c r="E79" s="81"/>
       <c r="F79" s="87"/>
@@ -5231,10 +5225,10 @@
       <c r="A80" s="26" t="s">
         <v>309</v>
       </c>
-      <c r="B80" s="211" t="s">
+      <c r="B80" s="220" t="s">
         <v>63</v>
       </c>
-      <c r="C80" s="212"/>
+      <c r="C80" s="221"/>
       <c r="D80" s="8"/>
       <c r="E80" s="81"/>
       <c r="F80" s="87"/>
@@ -5244,10 +5238,10 @@
       <c r="A81" s="26" t="s">
         <v>310</v>
       </c>
-      <c r="B81" s="211" t="s">
+      <c r="B81" s="220" t="s">
         <v>64</v>
       </c>
-      <c r="C81" s="212"/>
+      <c r="C81" s="221"/>
       <c r="D81" s="8"/>
       <c r="E81" s="81">
         <v>2</v>
@@ -5261,10 +5255,10 @@
       <c r="A82" s="26" t="s">
         <v>311</v>
       </c>
-      <c r="B82" s="211" t="s">
+      <c r="B82" s="220" t="s">
         <v>65</v>
       </c>
-      <c r="C82" s="212"/>
+      <c r="C82" s="221"/>
       <c r="D82" s="8"/>
       <c r="E82" s="81">
         <v>2</v>
@@ -5278,21 +5272,21 @@
       <c r="A83" s="27" t="s">
         <v>312</v>
       </c>
-      <c r="B83" s="209" t="s">
+      <c r="B83" s="224" t="s">
         <v>66</v>
       </c>
-      <c r="C83" s="210"/>
+      <c r="C83" s="225"/>
       <c r="D83" s="9"/>
       <c r="E83" s="88"/>
       <c r="F83" s="94"/>
       <c r="G83" s="46"/>
     </row>
     <row r="84" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B84" s="216" t="s">
+      <c r="B84" s="215" t="s">
         <v>67</v>
       </c>
-      <c r="C84" s="217"/>
-      <c r="D84" s="218"/>
+      <c r="C84" s="216"/>
+      <c r="D84" s="217"/>
       <c r="E84" s="84">
         <f>SUM(E77:E83)</f>
         <v>16</v>
@@ -5306,11 +5300,11 @@
       <c r="B85" s="1"/>
     </row>
     <row r="86" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B86" s="216" t="s">
+      <c r="B86" s="215" t="s">
         <v>68</v>
       </c>
-      <c r="C86" s="217"/>
-      <c r="D86" s="218"/>
+      <c r="C86" s="216"/>
+      <c r="D86" s="217"/>
       <c r="E86" s="84">
         <f>SUM(E70,E84)</f>
         <v>25</v>
@@ -5322,11 +5316,11 @@
     </row>
     <row r="87" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="88" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B88" s="216" t="s">
+      <c r="B88" s="215" t="s">
         <v>69</v>
       </c>
-      <c r="C88" s="217"/>
-      <c r="D88" s="218"/>
+      <c r="C88" s="216"/>
+      <c r="D88" s="217"/>
       <c r="E88" s="84">
         <f>SUM(E55,E86)</f>
         <v>40</v>
@@ -5344,12 +5338,12 @@
       <c r="A91" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="B91" s="213" t="str">
+      <c r="B91" s="234" t="str">
         <f>IF(AND(E91=0,F91=0),"Ok","Attention: The total liabilities do not match the total assets. Please verify the amounts to ensure accurate financial reporting!")</f>
         <v>Attention: The total liabilities do not match the total assets. Please verify the amounts to ensure accurate financial reporting!</v>
       </c>
-      <c r="C91" s="214"/>
-      <c r="D91" s="215"/>
+      <c r="C91" s="235"/>
+      <c r="D91" s="236"/>
       <c r="E91" s="84">
         <f>E88-E42</f>
         <v>-104</v>
@@ -5368,13 +5362,60 @@
     </row>
   </sheetData>
   <mergeCells count="77">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B91:D91"/>
+    <mergeCell ref="B84:D84"/>
+    <mergeCell ref="B86:D86"/>
+    <mergeCell ref="B88:D88"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B58:G58"/>
+    <mergeCell ref="B59:G59"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B73:G73"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B22:C22"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B14:C14"/>
@@ -5391,60 +5432,13 @@
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B73:G73"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B58:G58"/>
-    <mergeCell ref="B59:G59"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B91:D91"/>
-    <mergeCell ref="B84:D84"/>
-    <mergeCell ref="B86:D86"/>
-    <mergeCell ref="B88:D88"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B4:G4"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="B91">
@@ -5480,7 +5474,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="B12" sqref="B12:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -5498,14 +5492,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="237" t="s">
+      <c r="A1" s="240" t="s">
         <v>407</v>
       </c>
-      <c r="B1" s="237"/>
-      <c r="C1" s="237"/>
-      <c r="D1" s="237"/>
-      <c r="E1" s="237"/>
-      <c r="F1" s="238"/>
+      <c r="B1" s="240"/>
+      <c r="C1" s="240"/>
+      <c r="D1" s="240"/>
+      <c r="E1" s="240"/>
+      <c r="F1" s="241"/>
       <c r="G1" s="126"/>
       <c r="H1" s="126"/>
       <c r="I1" s="126"/>
@@ -5514,53 +5508,53 @@
       <c r="A2" s="136" t="s">
         <v>423</v>
       </c>
-      <c r="B2" s="197" t="str">
+      <c r="B2" s="194" t="str">
         <f>'General information'!B2</f>
         <v>CompanyName LegalForm</v>
       </c>
-      <c r="C2" s="198"/>
-      <c r="D2" s="198"/>
-      <c r="E2" s="198"/>
-      <c r="F2" s="199"/>
+      <c r="C2" s="195"/>
+      <c r="D2" s="195"/>
+      <c r="E2" s="195"/>
+      <c r="F2" s="196"/>
     </row>
     <row r="3" spans="1:9" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="140" t="s">
         <v>426</v>
       </c>
-      <c r="B3" s="197" t="str">
+      <c r="B3" s="194" t="str">
         <f>'General information'!B3</f>
         <v>Address 1234, Country</v>
       </c>
-      <c r="C3" s="198"/>
-      <c r="D3" s="198"/>
-      <c r="E3" s="198"/>
-      <c r="F3" s="199"/>
+      <c r="C3" s="195"/>
+      <c r="D3" s="195"/>
+      <c r="E3" s="195"/>
+      <c r="F3" s="196"/>
     </row>
     <row r="4" spans="1:9" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="136" t="s">
         <v>80</v>
       </c>
-      <c r="B4" s="206">
+      <c r="B4" s="197">
         <f>'General information'!B8</f>
         <v>45291</v>
       </c>
-      <c r="C4" s="207"/>
-      <c r="D4" s="207"/>
-      <c r="E4" s="207"/>
-      <c r="F4" s="208"/>
+      <c r="C4" s="198"/>
+      <c r="D4" s="198"/>
+      <c r="E4" s="198"/>
+      <c r="F4" s="199"/>
     </row>
     <row r="5" spans="1:9" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="136" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="206">
+      <c r="B5" s="197">
         <f>'General information'!B9</f>
         <v>45657</v>
       </c>
-      <c r="C5" s="207"/>
-      <c r="D5" s="207"/>
-      <c r="E5" s="207"/>
-      <c r="F5" s="208"/>
+      <c r="C5" s="198"/>
+      <c r="D5" s="198"/>
+      <c r="E5" s="198"/>
+      <c r="F5" s="199"/>
     </row>
     <row r="6" spans="1:9" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="242" t="s">
@@ -5579,35 +5573,35 @@
       <c r="A7" s="128" t="s">
         <v>90</v>
       </c>
-      <c r="B7" s="239" t="s">
+      <c r="B7" s="237" t="s">
         <v>89</v>
       </c>
-      <c r="C7" s="240"/>
-      <c r="D7" s="240"/>
-      <c r="E7" s="240"/>
-      <c r="F7" s="241"/>
+      <c r="C7" s="238"/>
+      <c r="D7" s="238"/>
+      <c r="E7" s="238"/>
+      <c r="F7" s="239"/>
     </row>
     <row r="8" spans="1:9" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A8" s="129" t="s">
         <v>282</v>
       </c>
-      <c r="B8" s="239" t="s">
+      <c r="B8" s="237" t="s">
         <v>580</v>
       </c>
-      <c r="C8" s="240"/>
-      <c r="D8" s="240"/>
-      <c r="E8" s="240"/>
-      <c r="F8" s="241"/>
+      <c r="C8" s="238"/>
+      <c r="D8" s="238"/>
+      <c r="E8" s="238"/>
+      <c r="F8" s="239"/>
     </row>
     <row r="11" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="12" spans="1:9" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A12" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="B12" s="224" t="s">
+      <c r="B12" s="229" t="s">
         <v>71</v>
       </c>
-      <c r="C12" s="225"/>
+      <c r="C12" s="230"/>
       <c r="D12" s="179" t="s">
         <v>73</v>
       </c>
@@ -5624,13 +5618,13 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="216" t="s">
+      <c r="B13" s="215" t="s">
         <v>72</v>
       </c>
-      <c r="C13" s="217"/>
-      <c r="D13" s="217"/>
-      <c r="E13" s="217"/>
-      <c r="F13" s="217"/>
+      <c r="C13" s="216"/>
+      <c r="D13" s="216"/>
+      <c r="E13" s="216"/>
+      <c r="F13" s="216"/>
       <c r="G13" s="182"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -5813,10 +5807,10 @@
     </row>
     <row r="24" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="141"/>
-      <c r="B24" s="217" t="s">
+      <c r="B24" s="216" t="s">
         <v>290</v>
       </c>
-      <c r="C24" s="218"/>
+      <c r="C24" s="217"/>
       <c r="D24" s="143"/>
       <c r="E24" s="82">
         <f>SUM(E14:E23)</f>
@@ -5881,10 +5875,10 @@
     </row>
     <row r="28" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="141"/>
-      <c r="B28" s="217" t="s">
+      <c r="B28" s="216" t="s">
         <v>289</v>
       </c>
-      <c r="C28" s="218"/>
+      <c r="C28" s="217"/>
       <c r="D28" s="143"/>
       <c r="E28" s="82">
         <f>SUM(E24:E27)</f>
@@ -5914,10 +5908,10 @@
     </row>
     <row r="30" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="141"/>
-      <c r="B30" s="217" t="s">
+      <c r="B30" s="216" t="s">
         <v>408</v>
       </c>
-      <c r="C30" s="218"/>
+      <c r="C30" s="217"/>
       <c r="D30" s="143"/>
       <c r="E30" s="82">
         <f>SUM(E28:E29)</f>
@@ -5937,6 +5931,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="A6:F6"/>
     <mergeCell ref="B8:F8"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B12:C12"/>
@@ -5944,12 +5944,6 @@
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="B13:F13"/>
     <mergeCell ref="B24:C24"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="A6:F6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{9A9E6224-643C-4AD9-9436-A2DC070A0C83}"/>
@@ -5964,12 +5958,13 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B11" sqref="B11:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="40.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.7265625" customWidth="1"/>
+    <col min="2" max="2" width="40.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="111.08984375" customWidth="1"/>
     <col min="4" max="5" width="10.7265625" customWidth="1"/>
   </cols>
@@ -5989,79 +5984,79 @@
       <c r="A2" s="136" t="s">
         <v>423</v>
       </c>
-      <c r="B2" s="197" t="str">
+      <c r="B2" s="194" t="str">
         <f>'General information'!B2</f>
         <v>CompanyName LegalForm</v>
       </c>
-      <c r="C2" s="198"/>
-      <c r="D2" s="198"/>
-      <c r="E2" s="199"/>
+      <c r="C2" s="195"/>
+      <c r="D2" s="195"/>
+      <c r="E2" s="196"/>
     </row>
     <row r="3" spans="1:8" s="2" customFormat="1" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="140" t="s">
         <v>426</v>
       </c>
-      <c r="B3" s="197" t="str">
+      <c r="B3" s="194" t="str">
         <f>'General information'!B3</f>
         <v>Address 1234, Country</v>
       </c>
-      <c r="C3" s="198"/>
-      <c r="D3" s="198"/>
-      <c r="E3" s="199"/>
+      <c r="C3" s="195"/>
+      <c r="D3" s="195"/>
+      <c r="E3" s="196"/>
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="136" t="s">
         <v>80</v>
       </c>
-      <c r="B4" s="206">
+      <c r="B4" s="197">
         <f>'General information'!B8</f>
         <v>45291</v>
       </c>
-      <c r="C4" s="207"/>
-      <c r="D4" s="207"/>
-      <c r="E4" s="208"/>
+      <c r="C4" s="198"/>
+      <c r="D4" s="198"/>
+      <c r="E4" s="199"/>
     </row>
     <row r="5" spans="1:8" s="2" customFormat="1" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="136" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="206">
+      <c r="B5" s="197">
         <f>'General information'!B9</f>
         <v>45657</v>
       </c>
-      <c r="C5" s="207"/>
-      <c r="D5" s="207"/>
-      <c r="E5" s="208"/>
+      <c r="C5" s="198"/>
+      <c r="D5" s="198"/>
+      <c r="E5" s="199"/>
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="203" t="s">
+      <c r="B6" s="191" t="s">
         <v>406</v>
       </c>
-      <c r="C6" s="204"/>
-      <c r="D6" s="204"/>
-      <c r="E6" s="205"/>
+      <c r="C6" s="192"/>
+      <c r="D6" s="192"/>
+      <c r="E6" s="193"/>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="114" t="s">
         <v>90</v>
       </c>
-      <c r="B7" s="239" t="s">
+      <c r="B7" s="237" t="s">
         <v>89</v>
       </c>
-      <c r="C7" s="240"/>
-      <c r="D7" s="240"/>
-      <c r="E7" s="241"/>
+      <c r="C7" s="238"/>
+      <c r="D7" s="238"/>
+      <c r="E7" s="239"/>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A8" s="114" t="s">
         <v>282</v>
       </c>
-      <c r="B8" s="239" t="s">
+      <c r="B8" s="237" t="s">
         <v>581</v>
       </c>
-      <c r="C8" s="240"/>
-      <c r="D8" s="240"/>
-      <c r="E8" s="241"/>
+      <c r="C8" s="238"/>
+      <c r="D8" s="238"/>
+      <c r="E8" s="239"/>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6078,10 +6073,10 @@
       <c r="A11" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="B11" s="248" t="s">
+      <c r="B11" s="229" t="s">
         <v>389</v>
       </c>
-      <c r="C11" s="249"/>
+      <c r="C11" s="230"/>
       <c r="D11" s="113" t="s">
         <v>134</v>
       </c>
@@ -6308,117 +6303,117 @@
   </sheetPr>
   <dimension ref="A1:F92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G78" sqref="G78"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="40.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="125.7265625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.54296875" style="2" customWidth="1"/>
+    <col min="1" max="2" width="40.7265625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="129.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.6328125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7265625" style="2" customWidth="1"/>
     <col min="6" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="203" t="s">
+      <c r="B1" s="191" t="s">
         <v>407</v>
       </c>
-      <c r="C1" s="204"/>
-      <c r="D1" s="204"/>
-      <c r="E1" s="205"/>
+      <c r="C1" s="192"/>
+      <c r="D1" s="192"/>
+      <c r="E1" s="193"/>
       <c r="F1" s="126"/>
     </row>
     <row r="2" spans="1:6" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="136" t="s">
         <v>423</v>
       </c>
-      <c r="B2" s="197" t="str">
+      <c r="B2" s="194" t="str">
         <f>'General information'!B2</f>
         <v>CompanyName LegalForm</v>
       </c>
-      <c r="C2" s="198"/>
-      <c r="D2" s="198"/>
-      <c r="E2" s="199"/>
+      <c r="C2" s="195"/>
+      <c r="D2" s="195"/>
+      <c r="E2" s="196"/>
     </row>
     <row r="3" spans="1:6" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="140" t="s">
         <v>426</v>
       </c>
-      <c r="B3" s="197" t="str">
+      <c r="B3" s="194" t="str">
         <f>'General information'!B3</f>
         <v>Address 1234, Country</v>
       </c>
-      <c r="C3" s="198"/>
-      <c r="D3" s="198"/>
-      <c r="E3" s="199"/>
+      <c r="C3" s="195"/>
+      <c r="D3" s="195"/>
+      <c r="E3" s="196"/>
     </row>
     <row r="4" spans="1:6" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="136" t="s">
         <v>80</v>
       </c>
-      <c r="B4" s="206">
+      <c r="B4" s="197">
         <f>'General information'!B8</f>
         <v>45291</v>
       </c>
-      <c r="C4" s="207"/>
-      <c r="D4" s="207"/>
-      <c r="E4" s="208"/>
+      <c r="C4" s="198"/>
+      <c r="D4" s="198"/>
+      <c r="E4" s="199"/>
     </row>
     <row r="5" spans="1:6" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="136" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="206">
+      <c r="B5" s="197">
         <f>'General information'!B9</f>
         <v>45657</v>
       </c>
-      <c r="C5" s="207"/>
-      <c r="D5" s="207"/>
-      <c r="E5" s="208"/>
+      <c r="C5" s="198"/>
+      <c r="D5" s="198"/>
+      <c r="E5" s="199"/>
     </row>
     <row r="6" spans="1:6" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B6" s="203" t="s">
+      <c r="B6" s="191" t="s">
         <v>406</v>
       </c>
-      <c r="C6" s="204"/>
-      <c r="D6" s="204"/>
-      <c r="E6" s="205"/>
+      <c r="C6" s="192"/>
+      <c r="D6" s="192"/>
+      <c r="E6" s="193"/>
       <c r="F6" s="126"/>
     </row>
     <row r="7" spans="1:6" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="128" t="s">
         <v>90</v>
       </c>
-      <c r="B7" s="239" t="s">
+      <c r="B7" s="237" t="s">
         <v>89</v>
       </c>
-      <c r="C7" s="240"/>
-      <c r="D7" s="240"/>
-      <c r="E7" s="241"/>
+      <c r="C7" s="238"/>
+      <c r="D7" s="238"/>
+      <c r="E7" s="239"/>
     </row>
     <row r="8" spans="1:6" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A8" s="130" t="s">
         <v>282</v>
       </c>
-      <c r="B8" s="239" t="s">
+      <c r="B8" s="237" t="s">
         <v>582</v>
       </c>
-      <c r="C8" s="240"/>
-      <c r="D8" s="240"/>
-      <c r="E8" s="241"/>
+      <c r="C8" s="238"/>
+      <c r="D8" s="238"/>
+      <c r="E8" s="239"/>
     </row>
     <row r="9" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="10" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="250" t="s">
+      <c r="A10" s="253" t="s">
         <v>91</v>
       </c>
-      <c r="B10" s="252" t="s">
+      <c r="B10" s="255" t="s">
         <v>88</v>
       </c>
-      <c r="C10" s="253"/>
-      <c r="D10" s="259" t="s">
+      <c r="C10" s="256"/>
+      <c r="D10" s="248" t="s">
         <v>73</v>
       </c>
       <c r="E10" s="62">
@@ -6427,10 +6422,10 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="251"/>
-      <c r="B11" s="254"/>
-      <c r="C11" s="255"/>
-      <c r="D11" s="260"/>
+      <c r="A11" s="254"/>
+      <c r="B11" s="257"/>
+      <c r="C11" s="258"/>
+      <c r="D11" s="249"/>
       <c r="E11" s="62" t="s">
         <v>134</v>
       </c>
@@ -6439,21 +6434,21 @@
       <c r="A12" s="28" t="s">
         <v>457</v>
       </c>
-      <c r="B12" s="256" t="s">
+      <c r="B12" s="250" t="s">
         <v>383</v>
       </c>
-      <c r="C12" s="258"/>
-      <c r="D12" s="257"/>
+      <c r="C12" s="251"/>
+      <c r="D12" s="252"/>
       <c r="E12" s="96">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="256" t="s">
+      <c r="B13" s="250" t="s">
         <v>79</v>
       </c>
-      <c r="C13" s="258"/>
-      <c r="D13" s="257"/>
+      <c r="C13" s="251"/>
+      <c r="D13" s="252"/>
       <c r="E13" s="49"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -6743,10 +6738,10 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="256" t="s">
+      <c r="B36" s="250" t="s">
         <v>74</v>
       </c>
-      <c r="C36" s="258"/>
+      <c r="C36" s="251"/>
       <c r="D36" s="164"/>
       <c r="E36" s="100">
         <f>SUM(E14:E35)</f>
@@ -6840,22 +6835,22 @@
       <c r="F42" s="61"/>
     </row>
     <row r="43" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="256" t="s">
+      <c r="B43" s="250" t="s">
         <v>83</v>
       </c>
-      <c r="C43" s="258"/>
-      <c r="D43" s="257"/>
+      <c r="C43" s="251"/>
+      <c r="D43" s="252"/>
       <c r="E43" s="166">
         <f>E12+E36+SUM(E37:E42)</f>
         <v>17</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="256" t="s">
+      <c r="B44" s="250" t="s">
         <v>82</v>
       </c>
-      <c r="C44" s="258"/>
-      <c r="D44" s="257"/>
+      <c r="C44" s="251"/>
+      <c r="D44" s="252"/>
       <c r="E44" s="49"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -7104,22 +7099,22 @@
       <c r="E65" s="99"/>
     </row>
     <row r="66" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B66" s="256" t="s">
+      <c r="B66" s="250" t="s">
         <v>85</v>
       </c>
-      <c r="C66" s="258"/>
-      <c r="D66" s="257"/>
+      <c r="C66" s="251"/>
+      <c r="D66" s="252"/>
       <c r="E66" s="165">
         <f>SUM(E45:E65)</f>
         <v>89</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B67" s="256" t="s">
+      <c r="B67" s="250" t="s">
         <v>86</v>
       </c>
-      <c r="C67" s="258"/>
-      <c r="D67" s="257"/>
+      <c r="C67" s="251"/>
+      <c r="D67" s="252"/>
       <c r="E67" s="49"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -7261,22 +7256,22 @@
       <c r="E78" s="99"/>
     </row>
     <row r="79" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B79" s="256" t="s">
+      <c r="B79" s="250" t="s">
         <v>84</v>
       </c>
-      <c r="C79" s="258"/>
-      <c r="D79" s="257"/>
+      <c r="C79" s="251"/>
+      <c r="D79" s="252"/>
       <c r="E79" s="101">
         <f>SUM(E68:E78)</f>
         <v>12</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B80" s="256" t="s">
+      <c r="B80" s="250" t="s">
         <v>75</v>
       </c>
-      <c r="C80" s="258"/>
-      <c r="D80" s="257"/>
+      <c r="C80" s="251"/>
+      <c r="D80" s="252"/>
       <c r="E80" s="84">
         <f>SUM(E43,E66,E79)</f>
         <v>118</v>
@@ -7294,10 +7289,10 @@
       <c r="E81" s="99"/>
     </row>
     <row r="82" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B82" s="256" t="s">
+      <c r="B82" s="250" t="s">
         <v>76</v>
       </c>
-      <c r="C82" s="257"/>
+      <c r="C82" s="252"/>
       <c r="D82" s="171">
         <v>7.2</v>
       </c>
@@ -7307,33 +7302,33 @@
       </c>
     </row>
     <row r="83" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B83" s="256" t="s">
+      <c r="B83" s="250" t="s">
         <v>77</v>
       </c>
-      <c r="C83" s="258"/>
-      <c r="D83" s="257"/>
+      <c r="C83" s="251"/>
+      <c r="D83" s="252"/>
       <c r="E83" s="84">
         <f>'Statement of financial position'!E39</f>
         <v>10</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B84" s="256" t="s">
+      <c r="B84" s="250" t="s">
         <v>78</v>
       </c>
-      <c r="C84" s="258"/>
-      <c r="D84" s="257"/>
+      <c r="C84" s="251"/>
+      <c r="D84" s="252"/>
       <c r="E84" s="84">
         <f>'Statement of financial position'!F39</f>
         <v>15</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B85" s="256" t="s">
+      <c r="B85" s="250" t="s">
         <v>87</v>
       </c>
-      <c r="C85" s="258"/>
-      <c r="D85" s="257"/>
+      <c r="C85" s="251"/>
+      <c r="D85" s="252"/>
       <c r="E85" s="84">
         <f>E84-E83</f>
         <v>5</v>
@@ -7348,17 +7343,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:C11"/>
     <mergeCell ref="B82:C82"/>
@@ -7372,6 +7356,17 @@
     <mergeCell ref="B83:D83"/>
     <mergeCell ref="B80:D80"/>
     <mergeCell ref="B67:D67"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{5A53CF31-79B9-4E1F-A6DA-D8AE91352090}"/>
@@ -7389,8 +7384,8 @@
   </sheetPr>
   <dimension ref="A1:M249"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -7407,41 +7402,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="203" t="s">
+      <c r="A1" s="191" t="s">
         <v>407</v>
       </c>
-      <c r="B1" s="204"/>
-      <c r="C1" s="204"/>
-      <c r="D1" s="204"/>
-      <c r="E1" s="204"/>
-      <c r="F1" s="204"/>
-      <c r="G1" s="204"/>
-      <c r="H1" s="204"/>
-      <c r="I1" s="204"/>
-      <c r="J1" s="204"/>
-      <c r="K1" s="204"/>
-      <c r="L1" s="204"/>
-      <c r="M1" s="205"/>
+      <c r="B1" s="192"/>
+      <c r="C1" s="192"/>
+      <c r="D1" s="192"/>
+      <c r="E1" s="192"/>
+      <c r="F1" s="192"/>
+      <c r="G1" s="192"/>
+      <c r="H1" s="192"/>
+      <c r="I1" s="192"/>
+      <c r="J1" s="192"/>
+      <c r="K1" s="192"/>
+      <c r="L1" s="192"/>
+      <c r="M1" s="193"/>
     </row>
     <row r="2" spans="1:13" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="136" t="s">
         <v>423</v>
       </c>
-      <c r="B2" s="270" t="str">
+      <c r="B2" s="263" t="str">
         <f>'General information'!B2</f>
         <v>CompanyName LegalForm</v>
       </c>
-      <c r="C2" s="271"/>
-      <c r="D2" s="271"/>
-      <c r="E2" s="271"/>
-      <c r="F2" s="271"/>
-      <c r="G2" s="271"/>
-      <c r="H2" s="271"/>
-      <c r="I2" s="271"/>
-      <c r="J2" s="271"/>
-      <c r="K2" s="271"/>
-      <c r="L2" s="271"/>
-      <c r="M2" s="272"/>
+      <c r="C2" s="264"/>
+      <c r="D2" s="264"/>
+      <c r="E2" s="264"/>
+      <c r="F2" s="264"/>
+      <c r="G2" s="264"/>
+      <c r="H2" s="264"/>
+      <c r="I2" s="264"/>
+      <c r="J2" s="264"/>
+      <c r="K2" s="264"/>
+      <c r="L2" s="264"/>
+      <c r="M2" s="265"/>
     </row>
     <row r="3" spans="1:13" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="140" t="s">
@@ -7451,37 +7446,37 @@
         <f>'General information'!B3</f>
         <v>Address 1234, Country</v>
       </c>
-      <c r="C3" s="233"/>
-      <c r="D3" s="233"/>
-      <c r="E3" s="233"/>
-      <c r="F3" s="233"/>
-      <c r="G3" s="233"/>
-      <c r="H3" s="233"/>
-      <c r="I3" s="233"/>
-      <c r="J3" s="233"/>
-      <c r="K3" s="233"/>
-      <c r="L3" s="233"/>
-      <c r="M3" s="233"/>
+      <c r="C3" s="211"/>
+      <c r="D3" s="211"/>
+      <c r="E3" s="211"/>
+      <c r="F3" s="211"/>
+      <c r="G3" s="211"/>
+      <c r="H3" s="211"/>
+      <c r="I3" s="211"/>
+      <c r="J3" s="211"/>
+      <c r="K3" s="211"/>
+      <c r="L3" s="211"/>
+      <c r="M3" s="211"/>
     </row>
     <row r="4" spans="1:13" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="136" t="s">
         <v>80</v>
       </c>
-      <c r="B4" s="191">
+      <c r="B4" s="200">
         <f>'General information'!B8</f>
         <v>45291</v>
       </c>
-      <c r="C4" s="192"/>
-      <c r="D4" s="192"/>
-      <c r="E4" s="192"/>
-      <c r="F4" s="192"/>
-      <c r="G4" s="192"/>
-      <c r="H4" s="192"/>
-      <c r="I4" s="192"/>
-      <c r="J4" s="192"/>
-      <c r="K4" s="192"/>
-      <c r="L4" s="192"/>
-      <c r="M4" s="193"/>
+      <c r="C4" s="201"/>
+      <c r="D4" s="201"/>
+      <c r="E4" s="201"/>
+      <c r="F4" s="201"/>
+      <c r="G4" s="201"/>
+      <c r="H4" s="201"/>
+      <c r="I4" s="201"/>
+      <c r="J4" s="201"/>
+      <c r="K4" s="201"/>
+      <c r="L4" s="201"/>
+      <c r="M4" s="202"/>
     </row>
     <row r="5" spans="1:13" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="136" t="s">
@@ -7491,72 +7486,72 @@
         <f>'General information'!B9</f>
         <v>45657</v>
       </c>
-      <c r="C5" s="193"/>
-      <c r="D5" s="193"/>
-      <c r="E5" s="193"/>
-      <c r="F5" s="193"/>
-      <c r="G5" s="193"/>
-      <c r="H5" s="193"/>
-      <c r="I5" s="193"/>
-      <c r="J5" s="193"/>
-      <c r="K5" s="193"/>
-      <c r="L5" s="193"/>
-      <c r="M5" s="193"/>
+      <c r="C5" s="202"/>
+      <c r="D5" s="202"/>
+      <c r="E5" s="202"/>
+      <c r="F5" s="202"/>
+      <c r="G5" s="202"/>
+      <c r="H5" s="202"/>
+      <c r="I5" s="202"/>
+      <c r="J5" s="202"/>
+      <c r="K5" s="202"/>
+      <c r="L5" s="202"/>
+      <c r="M5" s="202"/>
     </row>
     <row r="6" spans="1:13" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="203" t="s">
+      <c r="A6" s="191" t="s">
         <v>406</v>
       </c>
-      <c r="B6" s="204"/>
-      <c r="C6" s="204"/>
-      <c r="D6" s="204"/>
-      <c r="E6" s="204"/>
-      <c r="F6" s="204"/>
-      <c r="G6" s="204"/>
-      <c r="H6" s="204"/>
-      <c r="I6" s="204"/>
-      <c r="J6" s="204"/>
-      <c r="K6" s="204"/>
-      <c r="L6" s="204"/>
-      <c r="M6" s="205"/>
+      <c r="B6" s="192"/>
+      <c r="C6" s="192"/>
+      <c r="D6" s="192"/>
+      <c r="E6" s="192"/>
+      <c r="F6" s="192"/>
+      <c r="G6" s="192"/>
+      <c r="H6" s="192"/>
+      <c r="I6" s="192"/>
+      <c r="J6" s="192"/>
+      <c r="K6" s="192"/>
+      <c r="L6" s="192"/>
+      <c r="M6" s="193"/>
     </row>
     <row r="7" spans="1:13" ht="18" x14ac:dyDescent="0.4">
       <c r="A7" s="131" t="s">
         <v>90</v>
       </c>
-      <c r="B7" s="200" t="s">
+      <c r="B7" s="206" t="s">
         <v>89</v>
       </c>
-      <c r="C7" s="201"/>
-      <c r="D7" s="201"/>
-      <c r="E7" s="201"/>
-      <c r="F7" s="201"/>
-      <c r="G7" s="201"/>
-      <c r="H7" s="201"/>
-      <c r="I7" s="201"/>
-      <c r="J7" s="201"/>
-      <c r="K7" s="201"/>
-      <c r="L7" s="201"/>
-      <c r="M7" s="202"/>
+      <c r="C7" s="207"/>
+      <c r="D7" s="207"/>
+      <c r="E7" s="207"/>
+      <c r="F7" s="207"/>
+      <c r="G7" s="207"/>
+      <c r="H7" s="207"/>
+      <c r="I7" s="207"/>
+      <c r="J7" s="207"/>
+      <c r="K7" s="207"/>
+      <c r="L7" s="207"/>
+      <c r="M7" s="208"/>
     </row>
     <row r="8" spans="1:13" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A8" s="111" t="s">
         <v>282</v>
       </c>
-      <c r="B8" s="194" t="s">
+      <c r="B8" s="203" t="s">
         <v>583</v>
       </c>
-      <c r="C8" s="195"/>
-      <c r="D8" s="195"/>
-      <c r="E8" s="195"/>
-      <c r="F8" s="195"/>
-      <c r="G8" s="195"/>
-      <c r="H8" s="195"/>
-      <c r="I8" s="195"/>
-      <c r="J8" s="195"/>
-      <c r="K8" s="195"/>
-      <c r="L8" s="195"/>
-      <c r="M8" s="196"/>
+      <c r="C8" s="204"/>
+      <c r="D8" s="204"/>
+      <c r="E8" s="204"/>
+      <c r="F8" s="204"/>
+      <c r="G8" s="204"/>
+      <c r="H8" s="204"/>
+      <c r="I8" s="204"/>
+      <c r="J8" s="204"/>
+      <c r="K8" s="204"/>
+      <c r="L8" s="204"/>
+      <c r="M8" s="205"/>
     </row>
     <row r="9" spans="1:13" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
@@ -7564,21 +7559,21 @@
       <c r="C9" s="58"/>
     </row>
     <row r="10" spans="1:13" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="224" t="s">
+      <c r="A10" s="229" t="s">
         <v>294</v>
       </c>
-      <c r="B10" s="273"/>
-      <c r="C10" s="273"/>
-      <c r="D10" s="273"/>
-      <c r="E10" s="273"/>
-      <c r="F10" s="273"/>
-      <c r="G10" s="273"/>
-      <c r="H10" s="273"/>
-      <c r="I10" s="273"/>
-      <c r="J10" s="273"/>
-      <c r="K10" s="273"/>
-      <c r="L10" s="273"/>
-      <c r="M10" s="225"/>
+      <c r="B10" s="259"/>
+      <c r="C10" s="259"/>
+      <c r="D10" s="259"/>
+      <c r="E10" s="259"/>
+      <c r="F10" s="259"/>
+      <c r="G10" s="259"/>
+      <c r="H10" s="259"/>
+      <c r="I10" s="259"/>
+      <c r="J10" s="259"/>
+      <c r="K10" s="259"/>
+      <c r="L10" s="259"/>
+      <c r="M10" s="230"/>
     </row>
     <row r="11" spans="1:13" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="137" t="s">
@@ -7593,23 +7588,23 @@
       <c r="D11" s="132" t="s">
         <v>134</v>
       </c>
-      <c r="E11" s="267" t="s">
+      <c r="E11" s="260" t="s">
         <v>73</v>
       </c>
-      <c r="F11" s="268"/>
-      <c r="G11" s="268"/>
-      <c r="H11" s="268"/>
-      <c r="I11" s="268"/>
-      <c r="J11" s="268"/>
-      <c r="K11" s="268"/>
-      <c r="L11" s="268"/>
-      <c r="M11" s="269"/>
+      <c r="F11" s="261"/>
+      <c r="G11" s="261"/>
+      <c r="H11" s="261"/>
+      <c r="I11" s="261"/>
+      <c r="J11" s="261"/>
+      <c r="K11" s="261"/>
+      <c r="L11" s="261"/>
+      <c r="M11" s="262"/>
     </row>
     <row r="12" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="261" t="s">
+      <c r="A12" s="266" t="s">
         <v>427</v>
       </c>
-      <c r="B12" s="262"/>
+      <c r="B12" s="267"/>
       <c r="C12" s="65"/>
       <c r="D12" s="66"/>
       <c r="E12" s="66"/>
@@ -7920,10 +7915,10 @@
       <c r="B32" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="C32" s="221" t="s">
+      <c r="C32" s="226" t="s">
         <v>137</v>
       </c>
-      <c r="D32" s="223"/>
+      <c r="D32" s="228"/>
       <c r="E32" s="69" t="s">
         <v>400</v>
       </c>
@@ -8020,10 +8015,10 @@
     <row r="37" spans="1:13" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="19"/>
       <c r="B37" s="19"/>
-      <c r="C37" s="216" t="s">
+      <c r="C37" s="215" t="s">
         <v>142</v>
       </c>
-      <c r="D37" s="218"/>
+      <c r="D37" s="217"/>
       <c r="E37" s="69"/>
       <c r="F37" s="69"/>
       <c r="G37" s="69"/>
@@ -8313,10 +8308,10 @@
       <c r="B52" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C52" s="216" t="s">
+      <c r="C52" s="215" t="s">
         <v>3</v>
       </c>
-      <c r="D52" s="218"/>
+      <c r="D52" s="217"/>
       <c r="E52" s="68"/>
       <c r="F52" s="69"/>
       <c r="G52" s="69"/>
@@ -8406,10 +8401,10 @@
     <row r="57" spans="1:13" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="19"/>
       <c r="B57" s="19"/>
-      <c r="C57" s="216" t="s">
+      <c r="C57" s="215" t="s">
         <v>188</v>
       </c>
-      <c r="D57" s="218"/>
+      <c r="D57" s="217"/>
       <c r="E57" s="68"/>
       <c r="F57" s="69"/>
       <c r="G57" s="69"/>
@@ -8423,10 +8418,10 @@
     <row r="58" spans="1:13" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="19"/>
       <c r="B58" s="19"/>
-      <c r="C58" s="216" t="s">
+      <c r="C58" s="215" t="s">
         <v>187</v>
       </c>
-      <c r="D58" s="218"/>
+      <c r="D58" s="217"/>
       <c r="E58" s="68"/>
       <c r="F58" s="69"/>
       <c r="G58" s="69"/>
@@ -8656,10 +8651,10 @@
       <c r="B70" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C70" s="216" t="s">
+      <c r="C70" s="215" t="s">
         <v>21</v>
       </c>
-      <c r="D70" s="217"/>
+      <c r="D70" s="216"/>
       <c r="E70" s="68"/>
       <c r="F70" s="69"/>
       <c r="G70" s="69"/>
@@ -8959,21 +8954,21 @@
       <c r="M85" s="71"/>
     </row>
     <row r="86" spans="1:13" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="263" t="s">
+      <c r="A86" s="268" t="s">
         <v>294</v>
       </c>
-      <c r="B86" s="264"/>
-      <c r="C86" s="264"/>
-      <c r="D86" s="264"/>
-      <c r="E86" s="265"/>
-      <c r="F86" s="265"/>
-      <c r="G86" s="265"/>
-      <c r="H86" s="265"/>
-      <c r="I86" s="265"/>
-      <c r="J86" s="265"/>
-      <c r="K86" s="265"/>
-      <c r="L86" s="265"/>
-      <c r="M86" s="266"/>
+      <c r="B86" s="269"/>
+      <c r="C86" s="269"/>
+      <c r="D86" s="269"/>
+      <c r="E86" s="270"/>
+      <c r="F86" s="270"/>
+      <c r="G86" s="270"/>
+      <c r="H86" s="270"/>
+      <c r="I86" s="270"/>
+      <c r="J86" s="270"/>
+      <c r="K86" s="270"/>
+      <c r="L86" s="270"/>
+      <c r="M86" s="271"/>
     </row>
     <row r="87" spans="1:13" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="60" t="s">
@@ -8988,17 +8983,17 @@
       <c r="D87" s="59" t="s">
         <v>134</v>
       </c>
-      <c r="E87" s="267" t="s">
+      <c r="E87" s="260" t="s">
         <v>73</v>
       </c>
-      <c r="F87" s="268"/>
-      <c r="G87" s="268"/>
-      <c r="H87" s="268"/>
-      <c r="I87" s="268"/>
-      <c r="J87" s="268"/>
-      <c r="K87" s="268"/>
-      <c r="L87" s="268"/>
-      <c r="M87" s="269"/>
+      <c r="F87" s="261"/>
+      <c r="G87" s="261"/>
+      <c r="H87" s="261"/>
+      <c r="I87" s="261"/>
+      <c r="J87" s="261"/>
+      <c r="K87" s="261"/>
+      <c r="L87" s="261"/>
+      <c r="M87" s="262"/>
     </row>
     <row r="88" spans="1:13" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="56" t="s">
@@ -9024,10 +9019,10 @@
     <row r="89" spans="1:13" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="19"/>
       <c r="B89" s="29"/>
-      <c r="C89" s="216" t="s">
+      <c r="C89" s="215" t="s">
         <v>205</v>
       </c>
-      <c r="D89" s="218"/>
+      <c r="D89" s="217"/>
       <c r="E89" s="75"/>
       <c r="F89" s="76"/>
       <c r="G89" s="76"/>
@@ -9349,10 +9344,10 @@
     <row r="106" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A106" s="19"/>
       <c r="B106" s="19"/>
-      <c r="C106" s="217" t="s">
+      <c r="C106" s="216" t="s">
         <v>205</v>
       </c>
-      <c r="D106" s="218"/>
+      <c r="D106" s="217"/>
       <c r="E106" s="68"/>
       <c r="F106" s="69"/>
       <c r="G106" s="69"/>
@@ -9657,10 +9652,10 @@
       <c r="B122" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="C122" s="216" t="s">
+      <c r="C122" s="215" t="s">
         <v>61</v>
       </c>
-      <c r="D122" s="218"/>
+      <c r="D122" s="217"/>
       <c r="E122" s="65"/>
       <c r="F122" s="66"/>
       <c r="G122" s="66"/>
@@ -9750,10 +9745,10 @@
     <row r="127" spans="1:13" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A127" s="19"/>
       <c r="B127" s="19"/>
-      <c r="C127" s="216" t="s">
+      <c r="C127" s="215" t="s">
         <v>227</v>
       </c>
-      <c r="D127" s="218"/>
+      <c r="D127" s="217"/>
       <c r="E127" s="68"/>
       <c r="F127" s="69"/>
       <c r="G127" s="69"/>
@@ -9767,10 +9762,10 @@
     <row r="128" spans="1:13" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A128" s="19"/>
       <c r="B128" s="19"/>
-      <c r="C128" s="216" t="s">
+      <c r="C128" s="215" t="s">
         <v>228</v>
       </c>
-      <c r="D128" s="218"/>
+      <c r="D128" s="217"/>
       <c r="E128" s="68"/>
       <c r="F128" s="69"/>
       <c r="G128" s="69"/>
@@ -10115,10 +10110,10 @@
       <c r="B146" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="C146" s="216" t="s">
+      <c r="C146" s="215" t="s">
         <v>49</v>
       </c>
-      <c r="D146" s="218"/>
+      <c r="D146" s="217"/>
       <c r="E146" s="65"/>
       <c r="F146" s="66"/>
       <c r="G146" s="66"/>
@@ -10208,10 +10203,10 @@
     <row r="151" spans="1:13" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A151" s="19"/>
       <c r="B151" s="19"/>
-      <c r="C151" s="216" t="s">
+      <c r="C151" s="215" t="s">
         <v>249</v>
       </c>
-      <c r="D151" s="218"/>
+      <c r="D151" s="217"/>
       <c r="E151" s="68"/>
       <c r="F151" s="69"/>
       <c r="G151" s="69"/>
@@ -10225,10 +10220,10 @@
     <row r="152" spans="1:13" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A152" s="19"/>
       <c r="B152" s="19"/>
-      <c r="C152" s="216" t="s">
+      <c r="C152" s="215" t="s">
         <v>250</v>
       </c>
-      <c r="D152" s="218"/>
+      <c r="D152" s="217"/>
       <c r="E152" s="68"/>
       <c r="F152" s="69"/>
       <c r="G152" s="69"/>
@@ -10242,10 +10237,10 @@
     <row r="153" spans="1:13" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A153" s="19"/>
       <c r="B153" s="19"/>
-      <c r="C153" s="216" t="s">
+      <c r="C153" s="215" t="s">
         <v>251</v>
       </c>
-      <c r="D153" s="218"/>
+      <c r="D153" s="217"/>
       <c r="E153" s="68"/>
       <c r="F153" s="69"/>
       <c r="G153" s="69"/>
@@ -10552,10 +10547,10 @@
       <c r="B169" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="C169" s="216" t="s">
+      <c r="C169" s="215" t="s">
         <v>58</v>
       </c>
-      <c r="D169" s="218"/>
+      <c r="D169" s="217"/>
       <c r="E169" s="68"/>
       <c r="F169" s="69"/>
       <c r="G169" s="69"/>
@@ -10876,10 +10871,10 @@
       <c r="B187" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="C187" s="216" t="s">
+      <c r="C187" s="215" t="s">
         <v>46</v>
       </c>
-      <c r="D187" s="218"/>
+      <c r="D187" s="217"/>
       <c r="E187" s="68"/>
       <c r="F187" s="69"/>
       <c r="G187" s="69"/>
@@ -11151,10 +11146,10 @@
       <c r="B202" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="C202" s="216" t="s">
+      <c r="C202" s="215" t="s">
         <v>34</v>
       </c>
-      <c r="D202" s="218"/>
+      <c r="D202" s="217"/>
       <c r="E202" s="65"/>
       <c r="F202" s="66"/>
       <c r="G202" s="66"/>
@@ -11230,10 +11225,10 @@
       <c r="B206" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="C206" s="216" t="s">
+      <c r="C206" s="215" t="s">
         <v>258</v>
       </c>
-      <c r="D206" s="218"/>
+      <c r="D206" s="217"/>
       <c r="E206" s="65"/>
       <c r="F206" s="66"/>
       <c r="G206" s="66"/>
@@ -11872,10 +11867,10 @@
       <c r="B245" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="C245" s="216" t="s">
+      <c r="C245" s="215" t="s">
         <v>39</v>
       </c>
-      <c r="D245" s="217"/>
+      <c r="D245" s="216"/>
       <c r="E245" s="50"/>
       <c r="F245" s="52"/>
       <c r="G245" s="52"/>
@@ -11965,6 +11960,23 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="C169:D169"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C153:D153"/>
+    <mergeCell ref="C152:D152"/>
+    <mergeCell ref="C128:D128"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="A86:M86"/>
+    <mergeCell ref="E87:M87"/>
+    <mergeCell ref="C5:M5"/>
+    <mergeCell ref="B4:M4"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="C3:M3"/>
+    <mergeCell ref="B7:M7"/>
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="A6:M6"/>
     <mergeCell ref="C202:D202"/>
@@ -11981,23 +11993,6 @@
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="C37:D37"/>
     <mergeCell ref="B8:M8"/>
-    <mergeCell ref="C5:M5"/>
-    <mergeCell ref="B4:M4"/>
-    <mergeCell ref="B2:M2"/>
-    <mergeCell ref="C3:M3"/>
-    <mergeCell ref="B7:M7"/>
-    <mergeCell ref="C169:D169"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C153:D153"/>
-    <mergeCell ref="C152:D152"/>
-    <mergeCell ref="C128:D128"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="A86:M86"/>
-    <mergeCell ref="E87:M87"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{CAFC6D68-6070-4D51-BEF1-3FF68EC64F87}"/>
@@ -12015,8 +12010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB94D964-28C5-4002-956C-C8A9A1B2D354}">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12032,21 +12027,21 @@
       <c r="A1" s="136" t="s">
         <v>423</v>
       </c>
-      <c r="B1" s="270" t="str">
+      <c r="B1" s="263" t="str">
         <f>'General information'!B2</f>
         <v>CompanyName LegalForm</v>
       </c>
-      <c r="C1" s="271"/>
-      <c r="D1" s="271"/>
-      <c r="E1" s="271"/>
-      <c r="F1" s="271"/>
-      <c r="G1" s="271"/>
-      <c r="H1" s="271"/>
-      <c r="I1" s="271"/>
-      <c r="J1" s="271"/>
-      <c r="K1" s="271"/>
-      <c r="L1" s="271"/>
-      <c r="M1" s="272"/>
+      <c r="C1" s="264"/>
+      <c r="D1" s="264"/>
+      <c r="E1" s="264"/>
+      <c r="F1" s="264"/>
+      <c r="G1" s="264"/>
+      <c r="H1" s="264"/>
+      <c r="I1" s="264"/>
+      <c r="J1" s="264"/>
+      <c r="K1" s="264"/>
+      <c r="L1" s="264"/>
+      <c r="M1" s="265"/>
     </row>
     <row r="2" spans="1:13" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="140" t="s">
@@ -12056,37 +12051,37 @@
         <f>'General information'!B3</f>
         <v>Address 1234, Country</v>
       </c>
-      <c r="C2" s="233"/>
-      <c r="D2" s="233"/>
-      <c r="E2" s="233"/>
-      <c r="F2" s="233"/>
-      <c r="G2" s="233"/>
-      <c r="H2" s="233"/>
-      <c r="I2" s="233"/>
-      <c r="J2" s="233"/>
-      <c r="K2" s="233"/>
-      <c r="L2" s="233"/>
-      <c r="M2" s="233"/>
+      <c r="C2" s="211"/>
+      <c r="D2" s="211"/>
+      <c r="E2" s="211"/>
+      <c r="F2" s="211"/>
+      <c r="G2" s="211"/>
+      <c r="H2" s="211"/>
+      <c r="I2" s="211"/>
+      <c r="J2" s="211"/>
+      <c r="K2" s="211"/>
+      <c r="L2" s="211"/>
+      <c r="M2" s="211"/>
     </row>
     <row r="3" spans="1:13" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="136" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="191">
+      <c r="B3" s="200">
         <f>'General information'!B8</f>
         <v>45291</v>
       </c>
-      <c r="C3" s="192"/>
-      <c r="D3" s="192"/>
-      <c r="E3" s="192"/>
-      <c r="F3" s="192"/>
-      <c r="G3" s="192"/>
-      <c r="H3" s="192"/>
-      <c r="I3" s="192"/>
-      <c r="J3" s="192"/>
-      <c r="K3" s="192"/>
-      <c r="L3" s="192"/>
-      <c r="M3" s="193"/>
+      <c r="C3" s="201"/>
+      <c r="D3" s="201"/>
+      <c r="E3" s="201"/>
+      <c r="F3" s="201"/>
+      <c r="G3" s="201"/>
+      <c r="H3" s="201"/>
+      <c r="I3" s="201"/>
+      <c r="J3" s="201"/>
+      <c r="K3" s="201"/>
+      <c r="L3" s="201"/>
+      <c r="M3" s="202"/>
     </row>
     <row r="4" spans="1:13" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="136" t="s">
@@ -12096,90 +12091,90 @@
         <f>'General information'!B9</f>
         <v>45657</v>
       </c>
-      <c r="C4" s="193"/>
-      <c r="D4" s="193"/>
-      <c r="E4" s="193"/>
-      <c r="F4" s="193"/>
-      <c r="G4" s="193"/>
-      <c r="H4" s="193"/>
-      <c r="I4" s="193"/>
-      <c r="J4" s="193"/>
-      <c r="K4" s="193"/>
-      <c r="L4" s="193"/>
-      <c r="M4" s="193"/>
+      <c r="C4" s="202"/>
+      <c r="D4" s="202"/>
+      <c r="E4" s="202"/>
+      <c r="F4" s="202"/>
+      <c r="G4" s="202"/>
+      <c r="H4" s="202"/>
+      <c r="I4" s="202"/>
+      <c r="J4" s="202"/>
+      <c r="K4" s="202"/>
+      <c r="L4" s="202"/>
+      <c r="M4" s="202"/>
     </row>
     <row r="5" spans="1:13" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="203" t="s">
+      <c r="A5" s="191" t="s">
         <v>406</v>
       </c>
-      <c r="B5" s="204"/>
-      <c r="C5" s="204"/>
-      <c r="D5" s="204"/>
-      <c r="E5" s="204"/>
-      <c r="F5" s="204"/>
-      <c r="G5" s="204"/>
-      <c r="H5" s="204"/>
-      <c r="I5" s="204"/>
-      <c r="J5" s="204"/>
-      <c r="K5" s="204"/>
-      <c r="L5" s="204"/>
-      <c r="M5" s="205"/>
+      <c r="B5" s="192"/>
+      <c r="C5" s="192"/>
+      <c r="D5" s="192"/>
+      <c r="E5" s="192"/>
+      <c r="F5" s="192"/>
+      <c r="G5" s="192"/>
+      <c r="H5" s="192"/>
+      <c r="I5" s="192"/>
+      <c r="J5" s="192"/>
+      <c r="K5" s="192"/>
+      <c r="L5" s="192"/>
+      <c r="M5" s="193"/>
     </row>
     <row r="6" spans="1:13" ht="18" x14ac:dyDescent="0.4">
       <c r="A6" s="131" t="s">
         <v>90</v>
       </c>
-      <c r="B6" s="200" t="s">
+      <c r="B6" s="206" t="s">
         <v>89</v>
       </c>
-      <c r="C6" s="201"/>
-      <c r="D6" s="201"/>
-      <c r="E6" s="201"/>
-      <c r="F6" s="201"/>
-      <c r="G6" s="201"/>
-      <c r="H6" s="201"/>
-      <c r="I6" s="201"/>
-      <c r="J6" s="201"/>
-      <c r="K6" s="201"/>
-      <c r="L6" s="201"/>
-      <c r="M6" s="202"/>
+      <c r="C6" s="207"/>
+      <c r="D6" s="207"/>
+      <c r="E6" s="207"/>
+      <c r="F6" s="207"/>
+      <c r="G6" s="207"/>
+      <c r="H6" s="207"/>
+      <c r="I6" s="207"/>
+      <c r="J6" s="207"/>
+      <c r="K6" s="207"/>
+      <c r="L6" s="207"/>
+      <c r="M6" s="208"/>
     </row>
     <row r="7" spans="1:13" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="111" t="s">
         <v>282</v>
       </c>
-      <c r="B7" s="194" t="s">
+      <c r="B7" s="203" t="s">
         <v>584</v>
       </c>
-      <c r="C7" s="195"/>
-      <c r="D7" s="195"/>
-      <c r="E7" s="195"/>
-      <c r="F7" s="195"/>
-      <c r="G7" s="195"/>
-      <c r="H7" s="195"/>
-      <c r="I7" s="195"/>
-      <c r="J7" s="195"/>
-      <c r="K7" s="195"/>
-      <c r="L7" s="195"/>
-      <c r="M7" s="196"/>
+      <c r="C7" s="204"/>
+      <c r="D7" s="204"/>
+      <c r="E7" s="204"/>
+      <c r="F7" s="204"/>
+      <c r="G7" s="204"/>
+      <c r="H7" s="204"/>
+      <c r="I7" s="204"/>
+      <c r="J7" s="204"/>
+      <c r="K7" s="204"/>
+      <c r="L7" s="204"/>
+      <c r="M7" s="205"/>
     </row>
     <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="10" spans="1:13" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="224" t="s">
+      <c r="A10" s="229" t="s">
         <v>518</v>
       </c>
-      <c r="B10" s="273"/>
-      <c r="C10" s="273"/>
-      <c r="D10" s="273"/>
-      <c r="E10" s="273"/>
-      <c r="F10" s="273"/>
-      <c r="G10" s="273"/>
-      <c r="H10" s="273"/>
-      <c r="I10" s="273"/>
-      <c r="J10" s="273"/>
-      <c r="K10" s="273"/>
-      <c r="L10" s="273"/>
-      <c r="M10" s="225"/>
+      <c r="B10" s="259"/>
+      <c r="C10" s="259"/>
+      <c r="D10" s="259"/>
+      <c r="E10" s="259"/>
+      <c r="F10" s="259"/>
+      <c r="G10" s="259"/>
+      <c r="H10" s="259"/>
+      <c r="I10" s="259"/>
+      <c r="J10" s="259"/>
+      <c r="K10" s="259"/>
+      <c r="L10" s="259"/>
+      <c r="M10" s="230"/>
     </row>
     <row r="11" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="60" t="s">
@@ -12194,17 +12189,17 @@
       <c r="D11" s="59" t="s">
         <v>134</v>
       </c>
-      <c r="E11" s="263" t="s">
+      <c r="E11" s="268" t="s">
         <v>73</v>
       </c>
-      <c r="F11" s="264"/>
-      <c r="G11" s="264"/>
-      <c r="H11" s="264"/>
-      <c r="I11" s="264"/>
-      <c r="J11" s="264"/>
-      <c r="K11" s="264"/>
-      <c r="L11" s="264"/>
-      <c r="M11" s="274"/>
+      <c r="F11" s="269"/>
+      <c r="G11" s="269"/>
+      <c r="H11" s="269"/>
+      <c r="I11" s="269"/>
+      <c r="J11" s="269"/>
+      <c r="K11" s="269"/>
+      <c r="L11" s="269"/>
+      <c r="M11" s="272"/>
     </row>
     <row r="12" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="55" t="s">
@@ -12213,10 +12208,10 @@
       <c r="B12" s="55" t="s">
         <v>531</v>
       </c>
-      <c r="C12" s="275" t="s">
+      <c r="C12" s="273" t="s">
         <v>532</v>
       </c>
-      <c r="D12" s="276"/>
+      <c r="D12" s="274"/>
       <c r="E12" s="65"/>
       <c r="F12" s="66"/>
       <c r="G12" s="66"/>
@@ -12310,7 +12305,9 @@
       <c r="C17" s="34" t="s">
         <v>536</v>
       </c>
-      <c r="D17" s="81"/>
+      <c r="D17" s="81">
+        <v>1</v>
+      </c>
       <c r="E17" s="68"/>
       <c r="F17" s="69"/>
       <c r="G17" s="69"/>
@@ -12385,8 +12382,7 @@
         <v>540</v>
       </c>
       <c r="D21" s="88">
-        <f>SUM(D18:D20)</f>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E21" s="68"/>
       <c r="F21" s="69"/>
@@ -12406,7 +12402,7 @@
       </c>
       <c r="D22" s="149">
         <f>SUM(D13:D21)</f>
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="E22" s="68"/>
       <c r="F22" s="69"/>
@@ -12618,8 +12614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B93A2ED-056F-4720-99B4-8FAF3132C851}">
   <dimension ref="A1:M68"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12635,21 +12631,21 @@
       <c r="A1" s="136" t="s">
         <v>423</v>
       </c>
-      <c r="B1" s="270" t="str">
+      <c r="B1" s="263" t="str">
         <f>'General information'!B2</f>
         <v>CompanyName LegalForm</v>
       </c>
-      <c r="C1" s="271"/>
-      <c r="D1" s="271"/>
-      <c r="E1" s="271"/>
-      <c r="F1" s="271"/>
-      <c r="G1" s="271"/>
-      <c r="H1" s="271"/>
-      <c r="I1" s="271"/>
-      <c r="J1" s="271"/>
-      <c r="K1" s="271"/>
-      <c r="L1" s="271"/>
-      <c r="M1" s="272"/>
+      <c r="C1" s="264"/>
+      <c r="D1" s="264"/>
+      <c r="E1" s="264"/>
+      <c r="F1" s="264"/>
+      <c r="G1" s="264"/>
+      <c r="H1" s="264"/>
+      <c r="I1" s="264"/>
+      <c r="J1" s="264"/>
+      <c r="K1" s="264"/>
+      <c r="L1" s="264"/>
+      <c r="M1" s="265"/>
     </row>
     <row r="2" spans="1:13" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="140" t="s">
@@ -12659,37 +12655,37 @@
         <f>'General information'!B3</f>
         <v>Address 1234, Country</v>
       </c>
-      <c r="C2" s="233"/>
-      <c r="D2" s="233"/>
-      <c r="E2" s="233"/>
-      <c r="F2" s="233"/>
-      <c r="G2" s="233"/>
-      <c r="H2" s="233"/>
-      <c r="I2" s="233"/>
-      <c r="J2" s="233"/>
-      <c r="K2" s="233"/>
-      <c r="L2" s="233"/>
-      <c r="M2" s="233"/>
+      <c r="C2" s="211"/>
+      <c r="D2" s="211"/>
+      <c r="E2" s="211"/>
+      <c r="F2" s="211"/>
+      <c r="G2" s="211"/>
+      <c r="H2" s="211"/>
+      <c r="I2" s="211"/>
+      <c r="J2" s="211"/>
+      <c r="K2" s="211"/>
+      <c r="L2" s="211"/>
+      <c r="M2" s="211"/>
     </row>
     <row r="3" spans="1:13" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="136" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="191">
+      <c r="B3" s="200">
         <f>'General information'!B8</f>
         <v>45291</v>
       </c>
-      <c r="C3" s="192"/>
-      <c r="D3" s="192"/>
-      <c r="E3" s="192"/>
-      <c r="F3" s="192"/>
-      <c r="G3" s="192"/>
-      <c r="H3" s="192"/>
-      <c r="I3" s="192"/>
-      <c r="J3" s="192"/>
-      <c r="K3" s="192"/>
-      <c r="L3" s="192"/>
-      <c r="M3" s="193"/>
+      <c r="C3" s="201"/>
+      <c r="D3" s="201"/>
+      <c r="E3" s="201"/>
+      <c r="F3" s="201"/>
+      <c r="G3" s="201"/>
+      <c r="H3" s="201"/>
+      <c r="I3" s="201"/>
+      <c r="J3" s="201"/>
+      <c r="K3" s="201"/>
+      <c r="L3" s="201"/>
+      <c r="M3" s="202"/>
     </row>
     <row r="4" spans="1:13" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="136" t="s">
@@ -12699,90 +12695,90 @@
         <f>'General information'!B9</f>
         <v>45657</v>
       </c>
-      <c r="C4" s="193"/>
-      <c r="D4" s="193"/>
-      <c r="E4" s="193"/>
-      <c r="F4" s="193"/>
-      <c r="G4" s="193"/>
-      <c r="H4" s="193"/>
-      <c r="I4" s="193"/>
-      <c r="J4" s="193"/>
-      <c r="K4" s="193"/>
-      <c r="L4" s="193"/>
-      <c r="M4" s="193"/>
+      <c r="C4" s="202"/>
+      <c r="D4" s="202"/>
+      <c r="E4" s="202"/>
+      <c r="F4" s="202"/>
+      <c r="G4" s="202"/>
+      <c r="H4" s="202"/>
+      <c r="I4" s="202"/>
+      <c r="J4" s="202"/>
+      <c r="K4" s="202"/>
+      <c r="L4" s="202"/>
+      <c r="M4" s="202"/>
     </row>
     <row r="5" spans="1:13" ht="20.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="203" t="s">
+      <c r="A5" s="191" t="s">
         <v>406</v>
       </c>
-      <c r="B5" s="204"/>
-      <c r="C5" s="204"/>
-      <c r="D5" s="204"/>
-      <c r="E5" s="204"/>
-      <c r="F5" s="204"/>
-      <c r="G5" s="204"/>
-      <c r="H5" s="204"/>
-      <c r="I5" s="204"/>
-      <c r="J5" s="204"/>
-      <c r="K5" s="204"/>
-      <c r="L5" s="204"/>
-      <c r="M5" s="205"/>
+      <c r="B5" s="192"/>
+      <c r="C5" s="192"/>
+      <c r="D5" s="192"/>
+      <c r="E5" s="192"/>
+      <c r="F5" s="192"/>
+      <c r="G5" s="192"/>
+      <c r="H5" s="192"/>
+      <c r="I5" s="192"/>
+      <c r="J5" s="192"/>
+      <c r="K5" s="192"/>
+      <c r="L5" s="192"/>
+      <c r="M5" s="193"/>
     </row>
     <row r="6" spans="1:13" ht="18" x14ac:dyDescent="0.4">
       <c r="A6" s="131" t="s">
         <v>90</v>
       </c>
-      <c r="B6" s="200" t="s">
+      <c r="B6" s="206" t="s">
         <v>89</v>
       </c>
-      <c r="C6" s="201"/>
-      <c r="D6" s="201"/>
-      <c r="E6" s="201"/>
-      <c r="F6" s="201"/>
-      <c r="G6" s="201"/>
-      <c r="H6" s="201"/>
-      <c r="I6" s="201"/>
-      <c r="J6" s="201"/>
-      <c r="K6" s="201"/>
-      <c r="L6" s="201"/>
-      <c r="M6" s="202"/>
+      <c r="C6" s="207"/>
+      <c r="D6" s="207"/>
+      <c r="E6" s="207"/>
+      <c r="F6" s="207"/>
+      <c r="G6" s="207"/>
+      <c r="H6" s="207"/>
+      <c r="I6" s="207"/>
+      <c r="J6" s="207"/>
+      <c r="K6" s="207"/>
+      <c r="L6" s="207"/>
+      <c r="M6" s="208"/>
     </row>
     <row r="7" spans="1:13" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="111" t="s">
         <v>282</v>
       </c>
-      <c r="B7" s="194" t="s">
+      <c r="B7" s="203" t="s">
         <v>588</v>
       </c>
-      <c r="C7" s="195"/>
-      <c r="D7" s="195"/>
-      <c r="E7" s="195"/>
-      <c r="F7" s="195"/>
-      <c r="G7" s="195"/>
-      <c r="H7" s="195"/>
-      <c r="I7" s="195"/>
-      <c r="J7" s="195"/>
-      <c r="K7" s="195"/>
-      <c r="L7" s="195"/>
-      <c r="M7" s="196"/>
+      <c r="C7" s="204"/>
+      <c r="D7" s="204"/>
+      <c r="E7" s="204"/>
+      <c r="F7" s="204"/>
+      <c r="G7" s="204"/>
+      <c r="H7" s="204"/>
+      <c r="I7" s="204"/>
+      <c r="J7" s="204"/>
+      <c r="K7" s="204"/>
+      <c r="L7" s="204"/>
+      <c r="M7" s="205"/>
     </row>
     <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="10" spans="1:13" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="224" t="s">
+      <c r="A10" s="229" t="s">
         <v>561</v>
       </c>
-      <c r="B10" s="273"/>
-      <c r="C10" s="273"/>
-      <c r="D10" s="273"/>
-      <c r="E10" s="273"/>
-      <c r="F10" s="273"/>
-      <c r="G10" s="273"/>
-      <c r="H10" s="273"/>
-      <c r="I10" s="273"/>
-      <c r="J10" s="273"/>
-      <c r="K10" s="273"/>
-      <c r="L10" s="273"/>
-      <c r="M10" s="225"/>
+      <c r="B10" s="259"/>
+      <c r="C10" s="259"/>
+      <c r="D10" s="259"/>
+      <c r="E10" s="259"/>
+      <c r="F10" s="259"/>
+      <c r="G10" s="259"/>
+      <c r="H10" s="259"/>
+      <c r="I10" s="259"/>
+      <c r="J10" s="259"/>
+      <c r="K10" s="259"/>
+      <c r="L10" s="259"/>
+      <c r="M10" s="230"/>
     </row>
     <row r="11" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="137" t="s">
@@ -12797,17 +12793,17 @@
       <c r="D11" s="59" t="s">
         <v>134</v>
       </c>
-      <c r="E11" s="263" t="s">
+      <c r="E11" s="268" t="s">
         <v>73</v>
       </c>
-      <c r="F11" s="264"/>
-      <c r="G11" s="264"/>
-      <c r="H11" s="264"/>
-      <c r="I11" s="264"/>
-      <c r="J11" s="264"/>
-      <c r="K11" s="264"/>
-      <c r="L11" s="264"/>
-      <c r="M11" s="274"/>
+      <c r="F11" s="269"/>
+      <c r="G11" s="269"/>
+      <c r="H11" s="269"/>
+      <c r="I11" s="269"/>
+      <c r="J11" s="269"/>
+      <c r="K11" s="269"/>
+      <c r="L11" s="269"/>
+      <c r="M11" s="272"/>
     </row>
     <row r="12" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="182">
@@ -12816,10 +12812,10 @@
       <c r="B12" s="174" t="s">
         <v>565</v>
       </c>
-      <c r="C12" s="275" t="s">
+      <c r="C12" s="273" t="s">
         <v>565</v>
       </c>
-      <c r="D12" s="276"/>
+      <c r="D12" s="274"/>
       <c r="E12" s="65"/>
       <c r="F12" s="66"/>
       <c r="G12" s="66"/>
@@ -12912,11 +12908,11 @@
       <c r="A17" s="187">
         <v>7.2</v>
       </c>
-      <c r="B17" s="217" t="s">
+      <c r="B17" s="216" t="s">
         <v>570</v>
       </c>
-      <c r="C17" s="217"/>
-      <c r="D17" s="217"/>
+      <c r="C17" s="216"/>
+      <c r="D17" s="216"/>
       <c r="E17" s="65"/>
       <c r="F17" s="66"/>
       <c r="G17" s="66"/>
@@ -12971,7 +12967,9 @@
       <c r="C20" s="34" t="s">
         <v>572</v>
       </c>
-      <c r="D20" s="176"/>
+      <c r="D20" s="176">
+        <v>1</v>
+      </c>
       <c r="E20" s="68"/>
       <c r="F20" s="69"/>
       <c r="G20" s="69"/>
@@ -12990,7 +12988,7 @@
       </c>
       <c r="D21" s="177">
         <f>SUM(D18:D20)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E21" s="68"/>
       <c r="F21" s="69"/>
@@ -13006,10 +13004,10 @@
       <c r="A22" s="178">
         <v>7.21</v>
       </c>
-      <c r="B22" s="216" t="s">
+      <c r="B22" s="215" t="s">
         <v>574</v>
       </c>
-      <c r="C22" s="218"/>
+      <c r="C22" s="217"/>
       <c r="D22" s="49"/>
       <c r="E22" s="70"/>
       <c r="F22" s="11"/>
@@ -13733,18 +13731,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B7:M7"/>
+    <mergeCell ref="A10:M10"/>
+    <mergeCell ref="E11:M11"/>
+    <mergeCell ref="C12:D12"/>
     <mergeCell ref="B6:M6"/>
     <mergeCell ref="B1:M1"/>
     <mergeCell ref="C2:M2"/>
     <mergeCell ref="B3:M3"/>
     <mergeCell ref="C4:M4"/>
     <mergeCell ref="A5:M5"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B7:M7"/>
-    <mergeCell ref="A10:M10"/>
-    <mergeCell ref="E11:M11"/>
-    <mergeCell ref="C12:D12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" xr:uid="{DFD286F1-C21A-4D73-9C41-C9C69D815B5A}"/>

</xml_diff>